<commit_message>
Added SDE Problems sheet
</commit_message>
<xml_diff>
--- a/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1460,7 +1461,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1535,6 +1536,47 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1557,7 +1599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1584,6 +1626,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1891,7 +1944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1901,8 +1954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1935,230 +1988,230 @@
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="21">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="13" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2166,10 +2219,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="21">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2177,10 +2230,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="21">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2188,10 +2241,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="21">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2199,10 +2252,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="21">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2210,10 +2263,10 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="21">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -2221,10 +2274,10 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="21">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -2232,10 +2285,10 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="21">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2243,10 +2296,10 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="21">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -2254,10 +2307,10 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2265,10 +2318,10 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="21">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -2276,10 +2329,10 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="21">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2287,10 +2340,10 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="21">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2298,10 +2351,10 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="21">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2309,10 +2362,10 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2320,10 +2373,10 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="21">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -3337,76 +3390,76 @@
       <c r="C138" s="3"/>
     </row>
     <row r="139" spans="1:3" ht="21">
-      <c r="A139" s="7" t="s">
+      <c r="A139" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B139" s="5" t="s">
+      <c r="B139" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="C139" s="3" t="s">
-        <v>3</v>
+      <c r="C139" s="12" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">
-      <c r="A140" s="7" t="s">
+      <c r="A140" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B140" s="5" t="s">
+      <c r="B140" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C140" s="3" t="s">
-        <v>3</v>
+      <c r="C140" s="12" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21">
-      <c r="A141" s="7" t="s">
+      <c r="A141" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B141" s="5" t="s">
+      <c r="B141" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C141" s="3" t="s">
-        <v>3</v>
+      <c r="C141" s="12" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
-      <c r="A142" s="7" t="s">
+      <c r="A142" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B142" s="5" t="s">
+      <c r="B142" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="C142" s="3" t="s">
-        <v>3</v>
+      <c r="C142" s="12" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21">
-      <c r="A143" s="7" t="s">
+      <c r="A143" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B143" s="5" t="s">
+      <c r="B143" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C143" s="3" t="s">
-        <v>3</v>
+      <c r="C143" s="12" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21">
-      <c r="A144" s="7" t="s">
+      <c r="A144" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B144" s="5" t="s">
+      <c r="B144" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C144" s="3" t="s">
-        <v>3</v>
+      <c r="C144" s="12" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">
       <c r="A145" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B145" s="5" t="s">
+      <c r="B145" s="15" t="s">
         <v>140</v>
       </c>
       <c r="C145" s="3" t="s">
@@ -3417,7 +3470,7 @@
       <c r="A146" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B146" s="15" t="s">
         <v>141</v>
       </c>
       <c r="C146" s="3" t="s">
@@ -3428,7 +3481,7 @@
       <c r="A147" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B147" s="5" t="s">
+      <c r="B147" s="15" t="s">
         <v>142</v>
       </c>
       <c r="C147" s="3" t="s">
@@ -3439,7 +3492,7 @@
       <c r="A148" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B148" s="5" t="s">
+      <c r="B148" s="15" t="s">
         <v>143</v>
       </c>
       <c r="C148" s="3" t="s">
@@ -3450,7 +3503,7 @@
       <c r="A149" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B149" s="5" t="s">
+      <c r="B149" s="15" t="s">
         <v>144</v>
       </c>
       <c r="C149" s="3" t="s">
@@ -3461,7 +3514,7 @@
       <c r="A150" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="B150" s="15" t="s">
         <v>145</v>
       </c>
       <c r="C150" s="3" t="s">
@@ -3472,7 +3525,7 @@
       <c r="A151" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B151" s="5" t="s">
+      <c r="B151" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C151" s="3" t="s">
@@ -3483,7 +3536,7 @@
       <c r="A152" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B152" s="5" t="s">
+      <c r="B152" s="15" t="s">
         <v>147</v>
       </c>
       <c r="C152" s="3" t="s">
@@ -3494,7 +3547,7 @@
       <c r="A153" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B153" s="5" t="s">
+      <c r="B153" s="15" t="s">
         <v>148</v>
       </c>
       <c r="C153" s="3" t="s">
@@ -3505,7 +3558,7 @@
       <c r="A154" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="15" t="s">
         <v>149</v>
       </c>
       <c r="C154" s="3" t="s">
@@ -3516,7 +3569,7 @@
       <c r="A155" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B155" s="5" t="s">
+      <c r="B155" s="15" t="s">
         <v>150</v>
       </c>
       <c r="C155" s="3" t="s">
@@ -3527,7 +3580,7 @@
       <c r="A156" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B156" s="5" t="s">
+      <c r="B156" s="15" t="s">
         <v>151</v>
       </c>
       <c r="C156" s="3" t="s">
@@ -3538,7 +3591,7 @@
       <c r="A157" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B157" s="5" t="s">
+      <c r="B157" s="15" t="s">
         <v>152</v>
       </c>
       <c r="C157" s="3" t="s">
@@ -3549,7 +3602,7 @@
       <c r="A158" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B158" s="5" t="s">
+      <c r="B158" s="15" t="s">
         <v>153</v>
       </c>
       <c r="C158" s="3" t="s">
@@ -3560,7 +3613,7 @@
       <c r="A159" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B159" s="5" t="s">
+      <c r="B159" s="15" t="s">
         <v>154</v>
       </c>
       <c r="C159" s="3" t="s">
@@ -3571,7 +3624,7 @@
       <c r="A160" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B160" s="5" t="s">
+      <c r="B160" s="15" t="s">
         <v>155</v>
       </c>
       <c r="C160" s="3" t="s">
@@ -3582,7 +3635,7 @@
       <c r="A161" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B161" s="5" t="s">
+      <c r="B161" s="15" t="s">
         <v>156</v>
       </c>
       <c r="C161" s="3" t="s">
@@ -3593,7 +3646,7 @@
       <c r="A162" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B162" s="5" t="s">
+      <c r="B162" s="15" t="s">
         <v>157</v>
       </c>
       <c r="C162" s="3" t="s">
@@ -3604,7 +3657,7 @@
       <c r="A163" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B163" s="5" t="s">
+      <c r="B163" s="15" t="s">
         <v>158</v>
       </c>
       <c r="C163" s="3" t="s">
@@ -3615,7 +3668,7 @@
       <c r="A164" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B164" s="6" t="s">
+      <c r="B164" s="16" t="s">
         <v>159</v>
       </c>
       <c r="C164" s="3" t="s">
@@ -3626,7 +3679,7 @@
       <c r="A165" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B165" s="6" t="s">
+      <c r="B165" s="16" t="s">
         <v>160</v>
       </c>
       <c r="C165" s="3" t="s">
@@ -3637,7 +3690,7 @@
       <c r="A166" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B166" s="5" t="s">
+      <c r="B166" s="15" t="s">
         <v>161</v>
       </c>
       <c r="C166" s="3" t="s">
@@ -3648,7 +3701,7 @@
       <c r="A167" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B167" s="5" t="s">
+      <c r="B167" s="15" t="s">
         <v>162</v>
       </c>
       <c r="C167" s="3" t="s">
@@ -3659,7 +3712,7 @@
       <c r="A168" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B168" s="5" t="s">
+      <c r="B168" s="15" t="s">
         <v>163</v>
       </c>
       <c r="C168" s="3" t="s">
@@ -3670,7 +3723,7 @@
       <c r="A169" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B169" s="5" t="s">
+      <c r="B169" s="15" t="s">
         <v>164</v>
       </c>
       <c r="C169" s="3" t="s">
@@ -3681,7 +3734,7 @@
       <c r="A170" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B170" s="5" t="s">
+      <c r="B170" s="15" t="s">
         <v>165</v>
       </c>
       <c r="C170" s="3" t="s">
@@ -3692,7 +3745,7 @@
       <c r="A171" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B171" s="5" t="s">
+      <c r="B171" s="15" t="s">
         <v>166</v>
       </c>
       <c r="C171" s="3" t="s">
@@ -3703,7 +3756,7 @@
       <c r="A172" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B172" s="5" t="s">
+      <c r="B172" s="15" t="s">
         <v>167</v>
       </c>
       <c r="C172" s="3" t="s">
@@ -3714,7 +3767,7 @@
       <c r="A173" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B173" s="5" t="s">
+      <c r="B173" s="15" t="s">
         <v>168</v>
       </c>
       <c r="C173" s="3" t="s">
@@ -3725,7 +3778,7 @@
       <c r="A174" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B174" s="5" t="s">
+      <c r="B174" s="15" t="s">
         <v>169</v>
       </c>
       <c r="C174" s="3" t="s">

</xml_diff>

<commit_message>
modified SDE Preparation sheet
</commit_message>
<xml_diff>
--- a/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -1965,7 +1965,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1975,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C487"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B150" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3585,11 +3585,11 @@
       <c r="A154" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B154" s="12" t="s">
+      <c r="B154" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C154" s="3" t="s">
-        <v>3</v>
+      <c r="C154" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21">
@@ -3607,11 +3607,11 @@
       <c r="A156" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B156" s="12" t="s">
+      <c r="B156" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="C156" s="3" t="s">
-        <v>3</v>
+      <c r="C156" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="21">
@@ -3640,11 +3640,11 @@
       <c r="A159" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B159" s="12" t="s">
+      <c r="B159" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="C159" s="3" t="s">
-        <v>3</v>
+      <c r="C159" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Added/Modified problem status in Excel sheet
</commit_message>
<xml_diff>
--- a/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="468">
   <si>
     <t>Topic:</t>
   </si>
@@ -1455,13 +1455,22 @@
   </si>
   <si>
     <t>SDE PREPARATION SHEET FOR CODING ROUND BY WARUN SHARMA</t>
+  </si>
+  <si>
+    <t>Count occurences in a sorted array</t>
+  </si>
+  <si>
+    <t>Find peak element in an array</t>
+  </si>
+  <si>
+    <t>Median of two sorted array</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1594,6 +1603,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1616,7 +1642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1658,6 +1684,10 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1973,10 +2003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C487"/>
+  <dimension ref="A1:C490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3017,54 +3047,54 @@
       <c r="C100" s="3"/>
     </row>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B101" s="12" t="s">
+      <c r="B101" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>3</v>
+      <c r="C101" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="21">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B102" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>3</v>
+      <c r="C102" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B103" s="12" t="s">
+      <c r="B103" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="3" t="s">
-        <v>3</v>
+      <c r="C103" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="21">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B104" s="12" t="s">
+      <c r="B104" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>3</v>
+      <c r="C104" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B105" s="12" t="s">
+      <c r="B105" s="20" t="s">
         <v>101</v>
       </c>
       <c r="C105" s="3" t="s">
@@ -3072,7 +3102,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="21">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="19" t="s">
         <v>96</v>
       </c>
       <c r="B106" s="12" t="s">
@@ -3083,378 +3113,378 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="21">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B107" s="12" t="s">
+      <c r="B107" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>3</v>
+      <c r="C107" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="21">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B108" s="12" t="s">
+      <c r="B108" s="18" t="s">
+        <v>465</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="21">
+      <c r="A109" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B109" s="18" t="s">
+        <v>466</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="21">
+      <c r="A110" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B110" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="21">
-      <c r="A109" s="4" t="s">
+      <c r="C110" s="11" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="21">
+      <c r="A111" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B109" s="12" t="s">
+      <c r="B111" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="C111" s="11" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="21">
+      <c r="A112" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B112" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="21">
-      <c r="A110" s="4" t="s">
+      <c r="C112" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="21">
+      <c r="A113" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B110" s="12" t="s">
+      <c r="B113" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="21">
-      <c r="A111" s="4" t="s">
+      <c r="C113" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="21">
+      <c r="A114" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B111" s="12" t="s">
+      <c r="B114" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="21">
-      <c r="A112" s="4" t="s">
+      <c r="C114" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="21">
+      <c r="A115" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B112" s="12" t="s">
+      <c r="B115" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="21">
-      <c r="A113" s="4" t="s">
+      <c r="C115" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="21">
+      <c r="A116" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B113" s="12" t="s">
+      <c r="B116" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="21">
-      <c r="A114" s="4" t="s">
+      <c r="C116" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="21">
+      <c r="A117" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B114" s="12" t="s">
+      <c r="B117" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="21">
-      <c r="A115" s="4" t="s">
+      <c r="C117" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="21">
+      <c r="A118" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B115" s="12" t="s">
+      <c r="B118" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C115" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="21">
-      <c r="A116" s="4" t="s">
+      <c r="C118" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="21">
+      <c r="A119" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B116" s="12" t="s">
+      <c r="B119" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="21">
-      <c r="A117" s="4" t="s">
+      <c r="C119" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="21">
+      <c r="A120" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B117" s="12" t="s">
+      <c r="B120" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C117" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="21">
-      <c r="A118" s="4" t="s">
+      <c r="C120" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="21">
+      <c r="A121" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B118" s="12" t="s">
+      <c r="B121" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="21">
-      <c r="A119" s="4" t="s">
+      <c r="C121" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="21">
+      <c r="A122" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B119" s="12" t="s">
+      <c r="B122" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C119" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="21">
-      <c r="A120" s="4" t="s">
+      <c r="C122" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="21">
+      <c r="A123" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B120" s="12" t="s">
+      <c r="B123" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="21">
-      <c r="A121" s="4" t="s">
+      <c r="C123" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="21">
+      <c r="A124" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B121" s="12" t="s">
+      <c r="B124" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="21">
-      <c r="A122" s="4" t="s">
+      <c r="C124" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="21">
+      <c r="A125" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B122" s="12" t="s">
+      <c r="B125" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C122" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="21">
-      <c r="A123" s="4" t="s">
+      <c r="C125" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="21">
+      <c r="A126" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B123" s="12" t="s">
+      <c r="B126" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C123" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="21">
-      <c r="A124" s="4" t="s">
+      <c r="C126" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="21">
+      <c r="A127" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B124" s="12" t="s">
+      <c r="B127" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="21">
-      <c r="A125" s="4" t="s">
+      <c r="C127" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="21">
+      <c r="A128" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B125" s="12" t="s">
+      <c r="B128" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="21">
-      <c r="A126" s="4" t="s">
+      <c r="C128" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="21">
+      <c r="A129" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B126" s="12" t="s">
+      <c r="B129" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C126" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="21">
-      <c r="A127" s="4" t="s">
+      <c r="C129" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="21">
+      <c r="A130" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B127" s="12" t="s">
+      <c r="B130" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C127" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="21">
-      <c r="A128" s="4" t="s">
+      <c r="C130" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="21">
+      <c r="A131" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B128" s="12" t="s">
+      <c r="B131" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C128" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="21">
-      <c r="A129" s="4" t="s">
+      <c r="C131" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="21">
+      <c r="A132" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B129" s="12" t="s">
+      <c r="B132" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C129" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="21">
-      <c r="A130" s="4" t="s">
+      <c r="C132" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="21">
+      <c r="A133" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="B133" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C130" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="21">
-      <c r="A131" s="4" t="s">
+      <c r="C133" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="21">
+      <c r="A134" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B131" s="12" t="s">
+      <c r="B134" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C131" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="21">
-      <c r="A132" s="4" t="s">
+      <c r="C134" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="21">
+      <c r="A135" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B132" s="12" t="s">
+      <c r="B135" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C132" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="21">
-      <c r="A133" s="4" t="s">
+      <c r="C135" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="21">
+      <c r="A136" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B133" s="12" t="s">
+      <c r="B136" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C133" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="21">
-      <c r="A134" s="4" t="s">
+      <c r="C136" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="21">
+      <c r="A137" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B134" s="12" t="s">
+      <c r="B137" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C134" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="21">
-      <c r="A135" s="4" t="s">
+      <c r="C137" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="21">
+      <c r="A138" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B135" s="12" t="s">
+      <c r="B138" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C135" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="21">
-      <c r="A136" s="4" t="s">
+      <c r="C138" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="21">
+      <c r="A139" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B136" s="12" t="s">
+      <c r="B139" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C136" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="21">
-      <c r="B138" s="5"/>
-      <c r="C138" s="3"/>
-    </row>
-    <row r="139" spans="1:3" ht="21">
-      <c r="A139" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B139" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C139" s="10" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="21">
-      <c r="A140" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B140" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C140" s="10" t="s">
-        <v>463</v>
+      <c r="C139" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21">
-      <c r="A141" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B141" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="C141" s="10" t="s">
-        <v>463</v>
-      </c>
+      <c r="B141" s="5"/>
+      <c r="C141" s="3"/>
     </row>
     <row r="142" spans="1:3" ht="21">
       <c r="A142" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B142" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C142" s="10" t="s">
         <v>463</v>
@@ -3465,7 +3495,7 @@
         <v>133</v>
       </c>
       <c r="B143" s="18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C143" s="10" t="s">
         <v>463</v>
@@ -3476,40 +3506,40 @@
         <v>133</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C144" s="10" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">
-      <c r="A145" s="6" t="s">
+      <c r="A145" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B145" s="18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C145" s="10" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21">
-      <c r="A146" s="6" t="s">
+      <c r="A146" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B146" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C146" s="10" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21">
-      <c r="A147" s="6" t="s">
+      <c r="A147" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B147" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C147" s="10" t="s">
         <v>463</v>
@@ -3520,7 +3550,7 @@
         <v>133</v>
       </c>
       <c r="B148" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C148" s="10" t="s">
         <v>463</v>
@@ -3531,7 +3561,7 @@
         <v>133</v>
       </c>
       <c r="B149" s="18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C149" s="10" t="s">
         <v>463</v>
@@ -3542,7 +3572,7 @@
         <v>133</v>
       </c>
       <c r="B150" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C150" s="10" t="s">
         <v>463</v>
@@ -3552,22 +3582,22 @@
       <c r="A151" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B151" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>3</v>
+      <c r="B151" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C151" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21">
       <c r="A152" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B152" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>3</v>
+      <c r="B152" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C152" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="21">
@@ -3575,7 +3605,7 @@
         <v>133</v>
       </c>
       <c r="B153" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C153" s="10" t="s">
         <v>463</v>
@@ -3585,11 +3615,11 @@
       <c r="A154" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B154" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="C154" s="10" t="s">
-        <v>463</v>
+      <c r="B154" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21">
@@ -3597,7 +3627,7 @@
         <v>133</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>3</v>
@@ -3608,7 +3638,7 @@
         <v>133</v>
       </c>
       <c r="B156" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C156" s="10" t="s">
         <v>463</v>
@@ -3619,7 +3649,7 @@
         <v>133</v>
       </c>
       <c r="B157" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C157" s="10" t="s">
         <v>463</v>
@@ -3629,11 +3659,11 @@
       <c r="A158" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B158" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C158" s="10" t="s">
-        <v>463</v>
+      <c r="B158" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21">
@@ -3641,7 +3671,7 @@
         <v>133</v>
       </c>
       <c r="B159" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C159" s="10" t="s">
         <v>463</v>
@@ -3651,33 +3681,33 @@
       <c r="A160" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B160" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>3</v>
+      <c r="B160" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C160" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="21">
       <c r="A161" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B161" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>3</v>
+      <c r="B161" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C161" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="21">
       <c r="A162" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B162" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>3</v>
+      <c r="B162" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C162" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="21">
@@ -3685,7 +3715,7 @@
         <v>133</v>
       </c>
       <c r="B163" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>3</v>
@@ -3695,8 +3725,8 @@
       <c r="A164" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B164" s="13" t="s">
-        <v>159</v>
+      <c r="B164" s="12" t="s">
+        <v>156</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>3</v>
@@ -3706,8 +3736,8 @@
       <c r="A165" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B165" s="13" t="s">
-        <v>160</v>
+      <c r="B165" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>3</v>
@@ -3718,7 +3748,7 @@
         <v>133</v>
       </c>
       <c r="B166" s="12" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>3</v>
@@ -3728,8 +3758,8 @@
       <c r="A167" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B167" s="12" t="s">
-        <v>162</v>
+      <c r="B167" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>3</v>
@@ -3739,8 +3769,8 @@
       <c r="A168" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B168" s="12" t="s">
-        <v>163</v>
+      <c r="B168" s="13" t="s">
+        <v>160</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>3</v>
@@ -3751,7 +3781,7 @@
         <v>133</v>
       </c>
       <c r="B169" s="12" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C169" s="3" t="s">
         <v>3</v>
@@ -3762,7 +3792,7 @@
         <v>133</v>
       </c>
       <c r="B170" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>3</v>
@@ -3773,7 +3803,7 @@
         <v>133</v>
       </c>
       <c r="B171" s="12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C171" s="3" t="s">
         <v>3</v>
@@ -3784,7 +3814,7 @@
         <v>133</v>
       </c>
       <c r="B172" s="12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>3</v>
@@ -3795,7 +3825,7 @@
         <v>133</v>
       </c>
       <c r="B173" s="12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>3</v>
@@ -3806,55 +3836,55 @@
         <v>133</v>
       </c>
       <c r="B174" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="21">
+      <c r="A175" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B175" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="21">
+      <c r="A176" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B176" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="21">
+      <c r="A177" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B177" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C174" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="21">
-      <c r="B176" s="5"/>
-      <c r="C176" s="3"/>
-    </row>
-    <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B177" s="12" t="s">
-        <v>171</v>
-      </c>
       <c r="C177" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="21">
-      <c r="A178" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B178" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="179" spans="1:3" ht="21">
-      <c r="A179" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B179" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B179" s="5"/>
+      <c r="C179" s="3"/>
     </row>
     <row r="180" spans="1:3" ht="21">
       <c r="A180" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B180" s="12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>3</v>
@@ -3865,7 +3895,7 @@
         <v>170</v>
       </c>
       <c r="B181" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C181" s="3" t="s">
         <v>3</v>
@@ -3876,7 +3906,7 @@
         <v>170</v>
       </c>
       <c r="B182" s="12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C182" s="3" t="s">
         <v>3</v>
@@ -3887,7 +3917,7 @@
         <v>170</v>
       </c>
       <c r="B183" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>3</v>
@@ -3898,7 +3928,7 @@
         <v>170</v>
       </c>
       <c r="B184" s="12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>3</v>
@@ -3909,7 +3939,7 @@
         <v>170</v>
       </c>
       <c r="B185" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>3</v>
@@ -3920,7 +3950,7 @@
         <v>170</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>3</v>
@@ -3931,7 +3961,7 @@
         <v>170</v>
       </c>
       <c r="B187" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>3</v>
@@ -3942,7 +3972,7 @@
         <v>170</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>3</v>
@@ -3953,7 +3983,7 @@
         <v>170</v>
       </c>
       <c r="B189" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>3</v>
@@ -3964,7 +3994,7 @@
         <v>170</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>3</v>
@@ -3975,7 +4005,7 @@
         <v>170</v>
       </c>
       <c r="B191" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>3</v>
@@ -3986,7 +4016,7 @@
         <v>170</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>3</v>
@@ -3997,7 +4027,7 @@
         <v>170</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>3</v>
@@ -4008,7 +4038,7 @@
         <v>170</v>
       </c>
       <c r="B194" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>3</v>
@@ -4019,7 +4049,7 @@
         <v>170</v>
       </c>
       <c r="B195" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>3</v>
@@ -4030,7 +4060,7 @@
         <v>170</v>
       </c>
       <c r="B196" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>3</v>
@@ -4041,7 +4071,7 @@
         <v>170</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>3</v>
@@ -4052,7 +4082,7 @@
         <v>170</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>3</v>
@@ -4063,7 +4093,7 @@
         <v>170</v>
       </c>
       <c r="B199" s="12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>3</v>
@@ -4074,7 +4104,7 @@
         <v>170</v>
       </c>
       <c r="B200" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>3</v>
@@ -4085,7 +4115,7 @@
         <v>170</v>
       </c>
       <c r="B201" s="12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>3</v>
@@ -4096,7 +4126,7 @@
         <v>170</v>
       </c>
       <c r="B202" s="12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C202" s="3" t="s">
         <v>3</v>
@@ -4107,7 +4137,7 @@
         <v>170</v>
       </c>
       <c r="B203" s="12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>3</v>
@@ -4118,7 +4148,7 @@
         <v>170</v>
       </c>
       <c r="B204" s="12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>3</v>
@@ -4129,7 +4159,7 @@
         <v>170</v>
       </c>
       <c r="B205" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>3</v>
@@ -4140,7 +4170,7 @@
         <v>170</v>
       </c>
       <c r="B206" s="12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>3</v>
@@ -4151,7 +4181,7 @@
         <v>170</v>
       </c>
       <c r="B207" s="12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>3</v>
@@ -4162,7 +4192,7 @@
         <v>170</v>
       </c>
       <c r="B208" s="12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>3</v>
@@ -4173,7 +4203,7 @@
         <v>170</v>
       </c>
       <c r="B209" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>3</v>
@@ -4184,7 +4214,7 @@
         <v>170</v>
       </c>
       <c r="B210" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>3</v>
@@ -4195,61 +4225,61 @@
         <v>170</v>
       </c>
       <c r="B211" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="21">
-      <c r="A212" s="6"/>
-      <c r="B212" s="13"/>
-      <c r="C212" s="3"/>
+      <c r="A212" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B212" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="213" spans="1:3" ht="21">
-      <c r="A213" s="6"/>
-      <c r="B213" s="13"/>
-      <c r="C213" s="3"/>
+      <c r="A213" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B213" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="214" spans="1:3" ht="21">
       <c r="A214" s="4" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="B214" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="21">
-      <c r="A215" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B215" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A215" s="6"/>
+      <c r="B215" s="13"/>
+      <c r="C215" s="3"/>
     </row>
     <row r="216" spans="1:3" ht="21">
-      <c r="A216" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B216" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A216" s="6"/>
+      <c r="B216" s="13"/>
+      <c r="C216" s="3"/>
     </row>
     <row r="217" spans="1:3" ht="21">
       <c r="A217" s="4" t="s">
         <v>206</v>
       </c>
       <c r="B217" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>3</v>
@@ -4260,7 +4290,7 @@
         <v>206</v>
       </c>
       <c r="B218" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>3</v>
@@ -4271,7 +4301,7 @@
         <v>206</v>
       </c>
       <c r="B219" s="12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>3</v>
@@ -4281,8 +4311,8 @@
       <c r="A220" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B220" s="16" t="s">
-        <v>213</v>
+      <c r="B220" s="12" t="s">
+        <v>210</v>
       </c>
       <c r="C220" s="3" t="s">
         <v>3</v>
@@ -4293,7 +4323,7 @@
         <v>206</v>
       </c>
       <c r="B221" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>3</v>
@@ -4304,7 +4334,7 @@
         <v>206</v>
       </c>
       <c r="B222" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>3</v>
@@ -4314,8 +4344,8 @@
       <c r="A223" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B223" s="12" t="s">
-        <v>216</v>
+      <c r="B223" s="16" t="s">
+        <v>213</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>3</v>
@@ -4326,7 +4356,7 @@
         <v>206</v>
       </c>
       <c r="B224" s="12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>3</v>
@@ -4337,7 +4367,7 @@
         <v>206</v>
       </c>
       <c r="B225" s="12" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>3</v>
@@ -4348,7 +4378,7 @@
         <v>206</v>
       </c>
       <c r="B226" s="12" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>3</v>
@@ -4359,7 +4389,7 @@
         <v>206</v>
       </c>
       <c r="B227" s="12" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>3</v>
@@ -4370,7 +4400,7 @@
         <v>206</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C228" s="3" t="s">
         <v>3</v>
@@ -4381,7 +4411,7 @@
         <v>206</v>
       </c>
       <c r="B229" s="12" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>3</v>
@@ -4392,7 +4422,7 @@
         <v>206</v>
       </c>
       <c r="B230" s="12" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>3</v>
@@ -4403,7 +4433,7 @@
         <v>206</v>
       </c>
       <c r="B231" s="12" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>3</v>
@@ -4414,7 +4444,7 @@
         <v>206</v>
       </c>
       <c r="B232" s="12" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>3</v>
@@ -4425,7 +4455,7 @@
         <v>206</v>
       </c>
       <c r="B233" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>3</v>
@@ -4436,7 +4466,7 @@
         <v>206</v>
       </c>
       <c r="B234" s="12" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>3</v>
@@ -4447,59 +4477,59 @@
         <v>206</v>
       </c>
       <c r="B235" s="12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="21">
-      <c r="B236" s="13"/>
-      <c r="C236" s="3"/>
+      <c r="A236" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B236" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="237" spans="1:3" ht="21">
-      <c r="B237" s="13"/>
-      <c r="C237" s="3"/>
+      <c r="A237" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B237" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="238" spans="1:3" ht="21">
       <c r="A238" s="4" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B238" s="12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="21">
-      <c r="A239" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B239" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B239" s="13"/>
+      <c r="C239" s="3"/>
     </row>
     <row r="240" spans="1:3" ht="21">
-      <c r="A240" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B240" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="C240" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B240" s="13"/>
+      <c r="C240" s="3"/>
     </row>
     <row r="241" spans="1:3" ht="21">
       <c r="A241" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B241" s="12" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C241" s="3" t="s">
         <v>3</v>
@@ -4510,7 +4540,7 @@
         <v>229</v>
       </c>
       <c r="B242" s="12" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C242" s="3" t="s">
         <v>3</v>
@@ -4521,7 +4551,7 @@
         <v>229</v>
       </c>
       <c r="B243" s="12" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>3</v>
@@ -4532,7 +4562,7 @@
         <v>229</v>
       </c>
       <c r="B244" s="12" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>3</v>
@@ -4543,7 +4573,7 @@
         <v>229</v>
       </c>
       <c r="B245" s="12" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>3</v>
@@ -4554,7 +4584,7 @@
         <v>229</v>
       </c>
       <c r="B246" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>3</v>
@@ -4565,7 +4595,7 @@
         <v>229</v>
       </c>
       <c r="B247" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>3</v>
@@ -4576,7 +4606,7 @@
         <v>229</v>
       </c>
       <c r="B248" s="12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>3</v>
@@ -4587,7 +4617,7 @@
         <v>229</v>
       </c>
       <c r="B249" s="12" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>3</v>
@@ -4598,7 +4628,7 @@
         <v>229</v>
       </c>
       <c r="B250" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C250" s="3" t="s">
         <v>3</v>
@@ -4609,7 +4639,7 @@
         <v>229</v>
       </c>
       <c r="B251" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C251" s="3" t="s">
         <v>3</v>
@@ -4620,7 +4650,7 @@
         <v>229</v>
       </c>
       <c r="B252" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C252" s="3" t="s">
         <v>3</v>
@@ -4631,7 +4661,7 @@
         <v>229</v>
       </c>
       <c r="B253" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C253" s="3" t="s">
         <v>3</v>
@@ -4642,7 +4672,7 @@
         <v>229</v>
       </c>
       <c r="B254" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>3</v>
@@ -4653,7 +4683,7 @@
         <v>229</v>
       </c>
       <c r="B255" s="12" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>3</v>
@@ -4664,7 +4694,7 @@
         <v>229</v>
       </c>
       <c r="B256" s="12" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>3</v>
@@ -4675,7 +4705,7 @@
         <v>229</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>3</v>
@@ -4686,7 +4716,7 @@
         <v>229</v>
       </c>
       <c r="B258" s="12" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>3</v>
@@ -4697,7 +4727,7 @@
         <v>229</v>
       </c>
       <c r="B259" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>3</v>
@@ -4708,7 +4738,7 @@
         <v>229</v>
       </c>
       <c r="B260" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>3</v>
@@ -4719,7 +4749,7 @@
         <v>229</v>
       </c>
       <c r="B261" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>3</v>
@@ -4730,7 +4760,7 @@
         <v>229</v>
       </c>
       <c r="B262" s="12" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C262" s="3" t="s">
         <v>3</v>
@@ -4741,7 +4771,7 @@
         <v>229</v>
       </c>
       <c r="B263" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>3</v>
@@ -4752,7 +4782,7 @@
         <v>229</v>
       </c>
       <c r="B264" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C264" s="3" t="s">
         <v>3</v>
@@ -4763,7 +4793,7 @@
         <v>229</v>
       </c>
       <c r="B265" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>3</v>
@@ -4774,7 +4804,7 @@
         <v>229</v>
       </c>
       <c r="B266" s="12" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>3</v>
@@ -4785,7 +4815,7 @@
         <v>229</v>
       </c>
       <c r="B267" s="12" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>3</v>
@@ -4796,7 +4826,7 @@
         <v>229</v>
       </c>
       <c r="B268" s="12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C268" s="3" t="s">
         <v>3</v>
@@ -4807,7 +4837,7 @@
         <v>229</v>
       </c>
       <c r="B269" s="12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C269" s="3" t="s">
         <v>3</v>
@@ -4818,7 +4848,7 @@
         <v>229</v>
       </c>
       <c r="B270" s="12" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C270" s="3" t="s">
         <v>3</v>
@@ -4829,7 +4859,7 @@
         <v>229</v>
       </c>
       <c r="B271" s="12" t="s">
-        <v>86</v>
+        <v>260</v>
       </c>
       <c r="C271" s="3" t="s">
         <v>3</v>
@@ -4840,59 +4870,59 @@
         <v>229</v>
       </c>
       <c r="B272" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="21">
-      <c r="B273" s="13"/>
-      <c r="C273" s="3"/>
+      <c r="A273" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B273" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C273" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="274" spans="1:3" ht="21">
-      <c r="B274" s="13"/>
-      <c r="C274" s="3"/>
+      <c r="A274" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B274" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C274" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="275" spans="1:3" ht="21">
       <c r="A275" s="4" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="B275" s="12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="21">
-      <c r="A276" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B276" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="C276" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B276" s="13"/>
+      <c r="C276" s="3"/>
     </row>
     <row r="277" spans="1:3" ht="21">
-      <c r="A277" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B277" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="C277" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B277" s="13"/>
+      <c r="C277" s="3"/>
     </row>
     <row r="278" spans="1:3" ht="21">
       <c r="A278" s="4" t="s">
         <v>264</v>
       </c>
       <c r="B278" s="12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C278" s="3" t="s">
         <v>3</v>
@@ -4903,7 +4933,7 @@
         <v>264</v>
       </c>
       <c r="B279" s="12" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C279" s="3" t="s">
         <v>3</v>
@@ -4914,7 +4944,7 @@
         <v>264</v>
       </c>
       <c r="B280" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C280" s="3" t="s">
         <v>3</v>
@@ -4925,7 +4955,7 @@
         <v>264</v>
       </c>
       <c r="B281" s="12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C281" s="3" t="s">
         <v>3</v>
@@ -4936,7 +4966,7 @@
         <v>264</v>
       </c>
       <c r="B282" s="12" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>3</v>
@@ -4947,7 +4977,7 @@
         <v>264</v>
       </c>
       <c r="B283" s="12" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>3</v>
@@ -4958,7 +4988,7 @@
         <v>264</v>
       </c>
       <c r="B284" s="12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>3</v>
@@ -4969,7 +4999,7 @@
         <v>264</v>
       </c>
       <c r="B285" s="12" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C285" s="3" t="s">
         <v>3</v>
@@ -4980,7 +5010,7 @@
         <v>264</v>
       </c>
       <c r="B286" s="12" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C286" s="3" t="s">
         <v>3</v>
@@ -4991,7 +5021,7 @@
         <v>264</v>
       </c>
       <c r="B287" s="12" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C287" s="3" t="s">
         <v>3</v>
@@ -5002,7 +5032,7 @@
         <v>264</v>
       </c>
       <c r="B288" s="12" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>3</v>
@@ -5013,7 +5043,7 @@
         <v>264</v>
       </c>
       <c r="B289" s="12" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C289" s="3" t="s">
         <v>3</v>
@@ -5024,7 +5054,7 @@
         <v>264</v>
       </c>
       <c r="B290" s="12" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C290" s="3" t="s">
         <v>3</v>
@@ -5035,7 +5065,7 @@
         <v>264</v>
       </c>
       <c r="B291" s="12" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>3</v>
@@ -5046,7 +5076,7 @@
         <v>264</v>
       </c>
       <c r="B292" s="12" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>3</v>
@@ -5057,59 +5087,59 @@
         <v>264</v>
       </c>
       <c r="B293" s="12" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C293" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="21">
-      <c r="B294" s="13"/>
-      <c r="C294" s="3"/>
+      <c r="A294" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B294" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C294" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="295" spans="1:3" ht="21">
-      <c r="B295" s="13"/>
-      <c r="C295" s="3"/>
+      <c r="A295" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B295" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C295" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="296" spans="1:3" ht="21">
       <c r="A296" s="4" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="B296" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C296" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="21">
-      <c r="A297" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B297" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="C297" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B297" s="13"/>
+      <c r="C297" s="3"/>
     </row>
     <row r="298" spans="1:3" ht="21">
-      <c r="A298" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B298" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="C298" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B298" s="13"/>
+      <c r="C298" s="3"/>
     </row>
     <row r="299" spans="1:3" ht="21">
       <c r="A299" s="4" t="s">
         <v>284</v>
       </c>
       <c r="B299" s="12" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C299" s="3" t="s">
         <v>3</v>
@@ -5120,7 +5150,7 @@
         <v>284</v>
       </c>
       <c r="B300" s="12" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C300" s="3" t="s">
         <v>3</v>
@@ -5131,7 +5161,7 @@
         <v>284</v>
       </c>
       <c r="B301" s="12" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C301" s="3" t="s">
         <v>3</v>
@@ -5142,7 +5172,7 @@
         <v>284</v>
       </c>
       <c r="B302" s="12" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C302" s="3" t="s">
         <v>3</v>
@@ -5153,7 +5183,7 @@
         <v>284</v>
       </c>
       <c r="B303" s="12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C303" s="3" t="s">
         <v>3</v>
@@ -5164,7 +5194,7 @@
         <v>284</v>
       </c>
       <c r="B304" s="12" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C304" s="3" t="s">
         <v>3</v>
@@ -5175,7 +5205,7 @@
         <v>284</v>
       </c>
       <c r="B305" s="12" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C305" s="3" t="s">
         <v>3</v>
@@ -5186,7 +5216,7 @@
         <v>284</v>
       </c>
       <c r="B306" s="12" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C306" s="3" t="s">
         <v>3</v>
@@ -5197,7 +5227,7 @@
         <v>284</v>
       </c>
       <c r="B307" s="12" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C307" s="3" t="s">
         <v>3</v>
@@ -5208,7 +5238,7 @@
         <v>284</v>
       </c>
       <c r="B308" s="12" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C308" s="3" t="s">
         <v>3</v>
@@ -5218,8 +5248,8 @@
       <c r="A309" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B309" s="16" t="s">
-        <v>298</v>
+      <c r="B309" s="12" t="s">
+        <v>295</v>
       </c>
       <c r="C309" s="3" t="s">
         <v>3</v>
@@ -5230,7 +5260,7 @@
         <v>284</v>
       </c>
       <c r="B310" s="12" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C310" s="3" t="s">
         <v>3</v>
@@ -5241,7 +5271,7 @@
         <v>284</v>
       </c>
       <c r="B311" s="12" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C311" s="3" t="s">
         <v>3</v>
@@ -5251,8 +5281,8 @@
       <c r="A312" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B312" s="12" t="s">
-        <v>301</v>
+      <c r="B312" s="16" t="s">
+        <v>298</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>3</v>
@@ -5263,7 +5293,7 @@
         <v>284</v>
       </c>
       <c r="B313" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C313" s="3" t="s">
         <v>3</v>
@@ -5274,7 +5304,7 @@
         <v>284</v>
       </c>
       <c r="B314" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>3</v>
@@ -5285,7 +5315,7 @@
         <v>284</v>
       </c>
       <c r="B315" s="12" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>3</v>
@@ -5296,7 +5326,7 @@
         <v>284</v>
       </c>
       <c r="B316" s="12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C316" s="3" t="s">
         <v>3</v>
@@ -5307,7 +5337,7 @@
         <v>284</v>
       </c>
       <c r="B317" s="12" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>3</v>
@@ -5318,7 +5348,7 @@
         <v>284</v>
       </c>
       <c r="B318" s="12" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>3</v>
@@ -5329,7 +5359,7 @@
         <v>284</v>
       </c>
       <c r="B319" s="12" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>3</v>
@@ -5340,7 +5370,7 @@
         <v>284</v>
       </c>
       <c r="B320" s="12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C320" s="3" t="s">
         <v>3</v>
@@ -5351,7 +5381,7 @@
         <v>284</v>
       </c>
       <c r="B321" s="12" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C321" s="3" t="s">
         <v>3</v>
@@ -5362,7 +5392,7 @@
         <v>284</v>
       </c>
       <c r="B322" s="12" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C322" s="3" t="s">
         <v>3</v>
@@ -5373,7 +5403,7 @@
         <v>284</v>
       </c>
       <c r="B323" s="12" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C323" s="3" t="s">
         <v>3</v>
@@ -5384,7 +5414,7 @@
         <v>284</v>
       </c>
       <c r="B324" s="12" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C324" s="3" t="s">
         <v>3</v>
@@ -5395,7 +5425,7 @@
         <v>284</v>
       </c>
       <c r="B325" s="12" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C325" s="3" t="s">
         <v>3</v>
@@ -5406,7 +5436,7 @@
         <v>284</v>
       </c>
       <c r="B326" s="12" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>3</v>
@@ -5417,7 +5447,7 @@
         <v>284</v>
       </c>
       <c r="B327" s="12" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C327" s="3" t="s">
         <v>3</v>
@@ -5428,7 +5458,7 @@
         <v>284</v>
       </c>
       <c r="B328" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>3</v>
@@ -5439,7 +5469,7 @@
         <v>284</v>
       </c>
       <c r="B329" s="12" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C329" s="3" t="s">
         <v>3</v>
@@ -5450,7 +5480,7 @@
         <v>284</v>
       </c>
       <c r="B330" s="12" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C330" s="3" t="s">
         <v>3</v>
@@ -5461,7 +5491,7 @@
         <v>284</v>
       </c>
       <c r="B331" s="12" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C331" s="3" t="s">
         <v>3</v>
@@ -5472,7 +5502,7 @@
         <v>284</v>
       </c>
       <c r="B332" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>3</v>
@@ -5483,59 +5513,59 @@
         <v>284</v>
       </c>
       <c r="B333" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="C333" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" ht="21">
+      <c r="A334" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B334" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="C334" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" ht="21">
+      <c r="A335" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B335" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C335" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" ht="21">
+      <c r="A336" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B336" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="C333" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="334" spans="1:3" ht="21">
-      <c r="B334" s="13"/>
-      <c r="C334" s="3"/>
-    </row>
-    <row r="335" spans="1:3" ht="21">
-      <c r="B335" s="13"/>
-      <c r="C335" s="3"/>
-    </row>
-    <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="B336" s="12" t="s">
-        <v>324</v>
-      </c>
       <c r="C336" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="21">
-      <c r="A337" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="B337" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="C337" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B337" s="13"/>
+      <c r="C337" s="3"/>
     </row>
     <row r="338" spans="1:3" ht="21">
-      <c r="A338" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="B338" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="C338" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B338" s="13"/>
+      <c r="C338" s="3"/>
     </row>
     <row r="339" spans="1:3" ht="21">
       <c r="A339" s="6" t="s">
         <v>323</v>
       </c>
       <c r="B339" s="12" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C339" s="3" t="s">
         <v>3</v>
@@ -5546,7 +5576,7 @@
         <v>323</v>
       </c>
       <c r="B340" s="12" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C340" s="3" t="s">
         <v>3</v>
@@ -5557,7 +5587,7 @@
         <v>323</v>
       </c>
       <c r="B341" s="12" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C341" s="3" t="s">
         <v>3</v>
@@ -5568,7 +5598,7 @@
         <v>323</v>
       </c>
       <c r="B342" s="12" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C342" s="3" t="s">
         <v>3</v>
@@ -5579,7 +5609,7 @@
         <v>323</v>
       </c>
       <c r="B343" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C343" s="3" t="s">
         <v>3</v>
@@ -5589,8 +5619,8 @@
       <c r="A344" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B344" s="16" t="s">
-        <v>332</v>
+      <c r="B344" s="12" t="s">
+        <v>329</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>3</v>
@@ -5601,7 +5631,7 @@
         <v>323</v>
       </c>
       <c r="B345" s="12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C345" s="3" t="s">
         <v>3</v>
@@ -5612,7 +5642,7 @@
         <v>323</v>
       </c>
       <c r="B346" s="12" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C346" s="3" t="s">
         <v>3</v>
@@ -5622,8 +5652,8 @@
       <c r="A347" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B347" s="12" t="s">
-        <v>335</v>
+      <c r="B347" s="16" t="s">
+        <v>332</v>
       </c>
       <c r="C347" s="3" t="s">
         <v>3</v>
@@ -5634,7 +5664,7 @@
         <v>323</v>
       </c>
       <c r="B348" s="12" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C348" s="3" t="s">
         <v>3</v>
@@ -5645,7 +5675,7 @@
         <v>323</v>
       </c>
       <c r="B349" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>3</v>
@@ -5656,7 +5686,7 @@
         <v>323</v>
       </c>
       <c r="B350" s="12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C350" s="3" t="s">
         <v>3</v>
@@ -5667,7 +5697,7 @@
         <v>323</v>
       </c>
       <c r="B351" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C351" s="3" t="s">
         <v>3</v>
@@ -5678,7 +5708,7 @@
         <v>323</v>
       </c>
       <c r="B352" s="12" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C352" s="3" t="s">
         <v>3</v>
@@ -5689,59 +5719,59 @@
         <v>323</v>
       </c>
       <c r="B353" s="12" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C353" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="354" spans="1:3" ht="21">
-      <c r="B354" s="13"/>
-      <c r="C354" s="3"/>
+      <c r="A354" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B354" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="C354" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="355" spans="1:3" ht="21">
-      <c r="B355" s="13"/>
-      <c r="C355" s="3"/>
+      <c r="A355" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B355" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="C355" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="6" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="B356" s="12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="21">
-      <c r="A357" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="B357" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="C357" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B357" s="13"/>
+      <c r="C357" s="3"/>
     </row>
     <row r="358" spans="1:3" ht="21">
-      <c r="A358" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="B358" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="C358" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B358" s="13"/>
+      <c r="C358" s="3"/>
     </row>
     <row r="359" spans="1:3" ht="21">
       <c r="A359" s="6" t="s">
         <v>342</v>
       </c>
       <c r="B359" s="12" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C359" s="3" t="s">
         <v>3</v>
@@ -5752,7 +5782,7 @@
         <v>342</v>
       </c>
       <c r="B360" s="12" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C360" s="3" t="s">
         <v>3</v>
@@ -5763,7 +5793,7 @@
         <v>342</v>
       </c>
       <c r="B361" s="12" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C361" s="3" t="s">
         <v>3</v>
@@ -5774,7 +5804,7 @@
         <v>342</v>
       </c>
       <c r="B362" s="12" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C362" s="3" t="s">
         <v>3</v>
@@ -5785,7 +5815,7 @@
         <v>342</v>
       </c>
       <c r="B363" s="12" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C363" s="3" t="s">
         <v>3</v>
@@ -5796,7 +5826,7 @@
         <v>342</v>
       </c>
       <c r="B364" s="12" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C364" s="3" t="s">
         <v>3</v>
@@ -5807,7 +5837,7 @@
         <v>342</v>
       </c>
       <c r="B365" s="12" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C365" s="3" t="s">
         <v>3</v>
@@ -5818,7 +5848,7 @@
         <v>342</v>
       </c>
       <c r="B366" s="12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C366" s="3" t="s">
         <v>3</v>
@@ -5829,7 +5859,7 @@
         <v>342</v>
       </c>
       <c r="B367" s="12" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C367" s="3" t="s">
         <v>3</v>
@@ -5840,7 +5870,7 @@
         <v>342</v>
       </c>
       <c r="B368" s="12" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C368" s="3" t="s">
         <v>3</v>
@@ -5851,7 +5881,7 @@
         <v>342</v>
       </c>
       <c r="B369" s="12" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C369" s="3" t="s">
         <v>3</v>
@@ -5862,7 +5892,7 @@
         <v>342</v>
       </c>
       <c r="B370" s="12" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C370" s="3" t="s">
         <v>3</v>
@@ -5873,7 +5903,7 @@
         <v>342</v>
       </c>
       <c r="B371" s="12" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C371" s="3" t="s">
         <v>3</v>
@@ -5884,7 +5914,7 @@
         <v>342</v>
       </c>
       <c r="B372" s="12" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C372" s="3" t="s">
         <v>3</v>
@@ -5895,7 +5925,7 @@
         <v>342</v>
       </c>
       <c r="B373" s="12" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>3</v>
@@ -5906,7 +5936,7 @@
         <v>342</v>
       </c>
       <c r="B374" s="12" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>3</v>
@@ -5917,7 +5947,7 @@
         <v>342</v>
       </c>
       <c r="B375" s="12" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>3</v>
@@ -5928,7 +5958,7 @@
         <v>342</v>
       </c>
       <c r="B376" s="12" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>3</v>
@@ -5939,7 +5969,7 @@
         <v>342</v>
       </c>
       <c r="B377" s="12" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>3</v>
@@ -5950,7 +5980,7 @@
         <v>342</v>
       </c>
       <c r="B378" s="12" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C378" s="3" t="s">
         <v>3</v>
@@ -5961,7 +5991,7 @@
         <v>342</v>
       </c>
       <c r="B379" s="12" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C379" s="3" t="s">
         <v>3</v>
@@ -5972,7 +6002,7 @@
         <v>342</v>
       </c>
       <c r="B380" s="12" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C380" s="3" t="s">
         <v>3</v>
@@ -5983,7 +6013,7 @@
         <v>342</v>
       </c>
       <c r="B381" s="12" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C381" s="3" t="s">
         <v>3</v>
@@ -5994,7 +6024,7 @@
         <v>342</v>
       </c>
       <c r="B382" s="12" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C382" s="3" t="s">
         <v>3</v>
@@ -6005,7 +6035,7 @@
         <v>342</v>
       </c>
       <c r="B383" s="12" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C383" s="3" t="s">
         <v>3</v>
@@ -6016,7 +6046,7 @@
         <v>342</v>
       </c>
       <c r="B384" s="12" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C384" s="3" t="s">
         <v>3</v>
@@ -6027,7 +6057,7 @@
         <v>342</v>
       </c>
       <c r="B385" s="12" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C385" s="3" t="s">
         <v>3</v>
@@ -6038,7 +6068,7 @@
         <v>342</v>
       </c>
       <c r="B386" s="12" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C386" s="3" t="s">
         <v>3</v>
@@ -6049,7 +6079,7 @@
         <v>342</v>
       </c>
       <c r="B387" s="12" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C387" s="3" t="s">
         <v>3</v>
@@ -6060,7 +6090,7 @@
         <v>342</v>
       </c>
       <c r="B388" s="12" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C388" s="3" t="s">
         <v>3</v>
@@ -6071,7 +6101,7 @@
         <v>342</v>
       </c>
       <c r="B389" s="12" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C389" s="3" t="s">
         <v>3</v>
@@ -6082,7 +6112,7 @@
         <v>342</v>
       </c>
       <c r="B390" s="12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C390" s="3" t="s">
         <v>3</v>
@@ -6093,7 +6123,7 @@
         <v>342</v>
       </c>
       <c r="B391" s="12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C391" s="3" t="s">
         <v>3</v>
@@ -6104,7 +6134,7 @@
         <v>342</v>
       </c>
       <c r="B392" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C392" s="3" t="s">
         <v>3</v>
@@ -6115,7 +6145,7 @@
         <v>342</v>
       </c>
       <c r="B393" s="12" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C393" s="3" t="s">
         <v>3</v>
@@ -6126,7 +6156,7 @@
         <v>342</v>
       </c>
       <c r="B394" s="12" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C394" s="3" t="s">
         <v>3</v>
@@ -6137,7 +6167,7 @@
         <v>342</v>
       </c>
       <c r="B395" s="12" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C395" s="3" t="s">
         <v>3</v>
@@ -6148,7 +6178,7 @@
         <v>342</v>
       </c>
       <c r="B396" s="12" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C396" s="3" t="s">
         <v>3</v>
@@ -6159,7 +6189,7 @@
         <v>342</v>
       </c>
       <c r="B397" s="12" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C397" s="3" t="s">
         <v>3</v>
@@ -6170,7 +6200,7 @@
         <v>342</v>
       </c>
       <c r="B398" s="12" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C398" s="3" t="s">
         <v>3</v>
@@ -6181,59 +6211,59 @@
         <v>342</v>
       </c>
       <c r="B399" s="12" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C399" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="400" spans="1:3" ht="21">
-      <c r="B400" s="13"/>
-      <c r="C400" s="3"/>
+      <c r="A400" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B400" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C400" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="401" spans="1:3" ht="21">
-      <c r="B401" s="13"/>
-      <c r="C401" s="3"/>
+      <c r="A401" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B401" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="C401" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="402" spans="1:3" ht="21">
       <c r="A402" s="6" t="s">
-        <v>386</v>
+        <v>342</v>
       </c>
       <c r="B402" s="12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C402" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="21">
-      <c r="A403" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B403" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="C403" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B403" s="13"/>
+      <c r="C403" s="3"/>
     </row>
     <row r="404" spans="1:3" ht="21">
-      <c r="A404" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B404" s="12" t="s">
-        <v>389</v>
-      </c>
-      <c r="C404" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B404" s="13"/>
+      <c r="C404" s="3"/>
     </row>
     <row r="405" spans="1:3" ht="21">
       <c r="A405" s="6" t="s">
         <v>386</v>
       </c>
       <c r="B405" s="12" t="s">
-        <v>88</v>
+        <v>387</v>
       </c>
       <c r="C405" s="3" t="s">
         <v>3</v>
@@ -6244,7 +6274,7 @@
         <v>386</v>
       </c>
       <c r="B406" s="12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C406" s="3" t="s">
         <v>3</v>
@@ -6255,59 +6285,59 @@
         <v>386</v>
       </c>
       <c r="B407" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="C407" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" ht="21">
+      <c r="A408" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B408" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C408" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" ht="21">
+      <c r="A409" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B409" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="C409" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" ht="21">
+      <c r="A410" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B410" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="C407" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="408" spans="1:3" ht="21">
-      <c r="B408" s="13"/>
-      <c r="C408" s="3"/>
-    </row>
-    <row r="409" spans="1:3" ht="21">
-      <c r="B409" s="13"/>
-      <c r="C409" s="3"/>
-    </row>
-    <row r="410" spans="1:3" ht="21">
-      <c r="A410" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B410" s="12" t="s">
-        <v>393</v>
-      </c>
       <c r="C410" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="21">
-      <c r="A411" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B411" s="12" t="s">
-        <v>394</v>
-      </c>
-      <c r="C411" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B411" s="13"/>
+      <c r="C411" s="3"/>
     </row>
     <row r="412" spans="1:3" ht="21">
-      <c r="A412" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B412" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="C412" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B412" s="13"/>
+      <c r="C412" s="3"/>
     </row>
     <row r="413" spans="1:3" ht="21">
       <c r="A413" s="4" t="s">
         <v>392</v>
       </c>
       <c r="B413" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C413" s="3" t="s">
         <v>3</v>
@@ -6318,7 +6348,7 @@
         <v>392</v>
       </c>
       <c r="B414" s="12" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C414" s="3" t="s">
         <v>3</v>
@@ -6329,7 +6359,7 @@
         <v>392</v>
       </c>
       <c r="B415" s="12" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C415" s="3" t="s">
         <v>3</v>
@@ -6340,7 +6370,7 @@
         <v>392</v>
       </c>
       <c r="B416" s="12" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C416" s="3" t="s">
         <v>3</v>
@@ -6351,7 +6381,7 @@
         <v>392</v>
       </c>
       <c r="B417" s="12" t="s">
-        <v>272</v>
+        <v>397</v>
       </c>
       <c r="C417" s="3" t="s">
         <v>3</v>
@@ -6362,7 +6392,7 @@
         <v>392</v>
       </c>
       <c r="B418" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C418" s="3" t="s">
         <v>3</v>
@@ -6373,7 +6403,7 @@
         <v>392</v>
       </c>
       <c r="B419" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C419" s="3" t="s">
         <v>3</v>
@@ -6384,7 +6414,7 @@
         <v>392</v>
       </c>
       <c r="B420" s="12" t="s">
-        <v>402</v>
+        <v>272</v>
       </c>
       <c r="C420" s="3" t="s">
         <v>3</v>
@@ -6395,7 +6425,7 @@
         <v>392</v>
       </c>
       <c r="B421" s="12" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C421" s="3" t="s">
         <v>3</v>
@@ -6406,7 +6436,7 @@
         <v>392</v>
       </c>
       <c r="B422" s="12" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C422" s="3" t="s">
         <v>3</v>
@@ -6417,7 +6447,7 @@
         <v>392</v>
       </c>
       <c r="B423" s="12" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C423" s="3" t="s">
         <v>3</v>
@@ -6428,7 +6458,7 @@
         <v>392</v>
       </c>
       <c r="B424" s="12" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C424" s="3" t="s">
         <v>3</v>
@@ -6439,7 +6469,7 @@
         <v>392</v>
       </c>
       <c r="B425" s="12" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C425" s="3" t="s">
         <v>3</v>
@@ -6450,7 +6480,7 @@
         <v>392</v>
       </c>
       <c r="B426" s="12" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C426" s="3" t="s">
         <v>3</v>
@@ -6461,7 +6491,7 @@
         <v>392</v>
       </c>
       <c r="B427" s="12" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C427" s="3" t="s">
         <v>3</v>
@@ -6472,7 +6502,7 @@
         <v>392</v>
       </c>
       <c r="B428" s="12" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C428" s="3" t="s">
         <v>3</v>
@@ -6483,7 +6513,7 @@
         <v>392</v>
       </c>
       <c r="B429" s="12" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C429" s="3" t="s">
         <v>3</v>
@@ -6494,7 +6524,7 @@
         <v>392</v>
       </c>
       <c r="B430" s="12" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C430" s="3" t="s">
         <v>3</v>
@@ -6505,7 +6535,7 @@
         <v>392</v>
       </c>
       <c r="B431" s="12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C431" s="3" t="s">
         <v>3</v>
@@ -6516,7 +6546,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="12" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C432" s="3" t="s">
         <v>3</v>
@@ -6527,7 +6557,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="12" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C433" s="3" t="s">
         <v>3</v>
@@ -6538,7 +6568,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="12" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C434" s="3" t="s">
         <v>3</v>
@@ -6549,7 +6579,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="12" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C435" s="3" t="s">
         <v>3</v>
@@ -6560,7 +6590,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="12" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C436" s="3" t="s">
         <v>3</v>
@@ -6571,7 +6601,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="12" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C437" s="3" t="s">
         <v>3</v>
@@ -6582,7 +6612,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="12" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C438" s="3" t="s">
         <v>3</v>
@@ -6593,7 +6623,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="12" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C439" s="3" t="s">
         <v>3</v>
@@ -6604,7 +6634,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="12" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C440" s="3" t="s">
         <v>3</v>
@@ -6615,7 +6645,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="12" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C441" s="3" t="s">
         <v>3</v>
@@ -6626,7 +6656,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="12" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C442" s="3" t="s">
         <v>3</v>
@@ -6637,7 +6667,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="12" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C443" s="3" t="s">
         <v>3</v>
@@ -6648,7 +6678,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="12" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C444" s="3" t="s">
         <v>3</v>
@@ -6659,7 +6689,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C445" s="3" t="s">
         <v>3</v>
@@ -6670,7 +6700,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="12" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C446" s="3" t="s">
         <v>3</v>
@@ -6681,7 +6711,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="12" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C447" s="3" t="s">
         <v>3</v>
@@ -6692,7 +6722,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="12" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C448" s="3" t="s">
         <v>3</v>
@@ -6703,7 +6733,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="12" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C449" s="3" t="s">
         <v>3</v>
@@ -6714,7 +6744,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="12" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C450" s="3" t="s">
         <v>3</v>
@@ -6725,7 +6755,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="12" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C451" s="3" t="s">
         <v>3</v>
@@ -6736,7 +6766,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="12" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C452" s="3" t="s">
         <v>3</v>
@@ -6747,7 +6777,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C453" s="3" t="s">
         <v>3</v>
@@ -6758,7 +6788,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="12" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C454" s="3" t="s">
         <v>3</v>
@@ -6769,7 +6799,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="12" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C455" s="3" t="s">
         <v>3</v>
@@ -6780,7 +6810,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="12" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C456" s="3" t="s">
         <v>3</v>
@@ -6791,7 +6821,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="12" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C457" s="3" t="s">
         <v>3</v>
@@ -6802,7 +6832,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="12" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C458" s="3" t="s">
         <v>3</v>
@@ -6813,7 +6843,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="12" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C459" s="3" t="s">
         <v>3</v>
@@ -6824,7 +6854,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="12" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C460" s="3" t="s">
         <v>3</v>
@@ -6835,7 +6865,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="12" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C461" s="3" t="s">
         <v>3</v>
@@ -6846,7 +6876,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="12" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C462" s="3" t="s">
         <v>3</v>
@@ -6857,7 +6887,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="12" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C463" s="3" t="s">
         <v>3</v>
@@ -6868,7 +6898,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="12" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C464" s="3" t="s">
         <v>3</v>
@@ -6879,7 +6909,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="12" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C465" s="3" t="s">
         <v>3</v>
@@ -6890,7 +6920,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="12" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C466" s="3" t="s">
         <v>3</v>
@@ -6901,7 +6931,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="12" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C467" s="3" t="s">
         <v>3</v>
@@ -6912,7 +6942,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="12" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C468" s="3" t="s">
         <v>3</v>
@@ -6923,60 +6953,60 @@
         <v>392</v>
       </c>
       <c r="B469" s="12" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C469" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="470" spans="1:3" ht="21">
-      <c r="B470" s="13"/>
-      <c r="C470" s="3"/>
+      <c r="A470" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B470" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="C470" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="471" spans="1:3" ht="21">
-      <c r="A471" s="6"/>
-      <c r="B471" s="13"/>
-      <c r="C471" s="3"/>
+      <c r="A471" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B471" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="C471" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="472" spans="1:3" ht="21">
       <c r="A472" s="4" t="s">
-        <v>452</v>
+        <v>392</v>
       </c>
       <c r="B472" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C472" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="473" spans="1:3" ht="21">
-      <c r="A473" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B473" s="12" t="s">
-        <v>454</v>
-      </c>
-      <c r="C473" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B473" s="13"/>
+      <c r="C473" s="3"/>
     </row>
     <row r="474" spans="1:3" ht="21">
-      <c r="A474" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B474" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="C474" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A474" s="6"/>
+      <c r="B474" s="13"/>
+      <c r="C474" s="3"/>
     </row>
     <row r="475" spans="1:3" ht="21">
       <c r="A475" s="4" t="s">
         <v>452</v>
       </c>
       <c r="B475" s="12" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C475" s="3" t="s">
         <v>3</v>
@@ -6987,7 +7017,7 @@
         <v>452</v>
       </c>
       <c r="B476" s="12" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C476" s="3" t="s">
         <v>3</v>
@@ -6998,7 +7028,7 @@
         <v>452</v>
       </c>
       <c r="B477" s="12" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C477" s="3" t="s">
         <v>3</v>
@@ -7009,7 +7039,7 @@
         <v>452</v>
       </c>
       <c r="B478" s="12" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C478" s="3" t="s">
         <v>3</v>
@@ -7020,7 +7050,7 @@
         <v>452</v>
       </c>
       <c r="B479" s="12" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C479" s="3" t="s">
         <v>3</v>
@@ -7031,7 +7061,7 @@
         <v>452</v>
       </c>
       <c r="B480" s="12" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C480" s="3" t="s">
         <v>3</v>
@@ -7042,20 +7072,44 @@
         <v>452</v>
       </c>
       <c r="B481" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="C481" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" ht="21">
+      <c r="A482" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B482" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="C482" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" ht="21">
+      <c r="A483" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B483" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="C483" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" ht="21">
+      <c r="A484" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B484" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="C481" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="482" spans="1:3">
-      <c r="B482" s="17"/>
-    </row>
-    <row r="483" spans="1:3">
-      <c r="B483" s="17"/>
-    </row>
-    <row r="484" spans="1:3">
-      <c r="B484" s="17"/>
+      <c r="C484" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="485" spans="1:3">
       <c r="B485" s="17"/>
@@ -7065,6 +7119,15 @@
     </row>
     <row r="487" spans="1:3">
       <c r="B487" s="17"/>
+    </row>
+    <row r="488" spans="1:3">
+      <c r="B488" s="17"/>
+    </row>
+    <row r="489" spans="1:3">
+      <c r="B489" s="17"/>
+    </row>
+    <row r="490" spans="1:3">
+      <c r="B490" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7162,360 +7225,362 @@
     <hyperlink ref="B104" r:id="rId92"/>
     <hyperlink ref="B106" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
     <hyperlink ref="B107" r:id="rId94"/>
-    <hyperlink ref="B108" r:id="rId95"/>
-    <hyperlink ref="B109" r:id="rId96"/>
-    <hyperlink ref="B110" r:id="rId97"/>
-    <hyperlink ref="B111" r:id="rId98"/>
-    <hyperlink ref="B113" r:id="rId99"/>
-    <hyperlink ref="B114" r:id="rId100"/>
-    <hyperlink ref="B115" r:id="rId101"/>
-    <hyperlink ref="B116" r:id="rId102"/>
-    <hyperlink ref="B117" r:id="rId103"/>
-    <hyperlink ref="B118" r:id="rId104"/>
-    <hyperlink ref="B119" r:id="rId105"/>
-    <hyperlink ref="B120" r:id="rId106"/>
-    <hyperlink ref="B121" r:id="rId107"/>
-    <hyperlink ref="B122" r:id="rId108"/>
-    <hyperlink ref="B123" r:id="rId109"/>
-    <hyperlink ref="B124" r:id="rId110"/>
-    <hyperlink ref="B125" r:id="rId111"/>
-    <hyperlink ref="B126" r:id="rId112"/>
-    <hyperlink ref="B127" r:id="rId113"/>
-    <hyperlink ref="B128" r:id="rId114"/>
-    <hyperlink ref="B129" r:id="rId115"/>
-    <hyperlink ref="B130" r:id="rId116"/>
-    <hyperlink ref="B131" r:id="rId117"/>
-    <hyperlink ref="B132" r:id="rId118"/>
-    <hyperlink ref="B133" r:id="rId119"/>
-    <hyperlink ref="B134" r:id="rId120"/>
-    <hyperlink ref="B135" r:id="rId121"/>
-    <hyperlink ref="B136" r:id="rId122"/>
+    <hyperlink ref="B110" r:id="rId95"/>
+    <hyperlink ref="B112" r:id="rId96"/>
+    <hyperlink ref="B113" r:id="rId97"/>
+    <hyperlink ref="B114" r:id="rId98"/>
+    <hyperlink ref="B116" r:id="rId99"/>
+    <hyperlink ref="B117" r:id="rId100"/>
+    <hyperlink ref="B118" r:id="rId101"/>
+    <hyperlink ref="B119" r:id="rId102"/>
+    <hyperlink ref="B120" r:id="rId103"/>
+    <hyperlink ref="B121" r:id="rId104"/>
+    <hyperlink ref="B122" r:id="rId105"/>
+    <hyperlink ref="B123" r:id="rId106"/>
+    <hyperlink ref="B124" r:id="rId107"/>
+    <hyperlink ref="B125" r:id="rId108"/>
+    <hyperlink ref="B126" r:id="rId109"/>
+    <hyperlink ref="B127" r:id="rId110"/>
+    <hyperlink ref="B128" r:id="rId111"/>
+    <hyperlink ref="B129" r:id="rId112"/>
+    <hyperlink ref="B130" r:id="rId113"/>
+    <hyperlink ref="B131" r:id="rId114"/>
+    <hyperlink ref="B132" r:id="rId115"/>
+    <hyperlink ref="B133" r:id="rId116"/>
+    <hyperlink ref="B134" r:id="rId117"/>
+    <hyperlink ref="B135" r:id="rId118"/>
+    <hyperlink ref="B136" r:id="rId119"/>
+    <hyperlink ref="B137" r:id="rId120"/>
+    <hyperlink ref="B138" r:id="rId121"/>
+    <hyperlink ref="B139" r:id="rId122"/>
     <hyperlink ref="B105" r:id="rId123"/>
-    <hyperlink ref="B112" r:id="rId124"/>
-    <hyperlink ref="B139" r:id="rId125"/>
-    <hyperlink ref="B140" r:id="rId126"/>
-    <hyperlink ref="B141" r:id="rId127"/>
-    <hyperlink ref="B142" r:id="rId128"/>
-    <hyperlink ref="B143" r:id="rId129"/>
-    <hyperlink ref="B144" r:id="rId130"/>
-    <hyperlink ref="B145" r:id="rId131"/>
-    <hyperlink ref="B146" r:id="rId132"/>
-    <hyperlink ref="B147" r:id="rId133"/>
-    <hyperlink ref="B148" r:id="rId134"/>
-    <hyperlink ref="B149" r:id="rId135"/>
-    <hyperlink ref="B150" r:id="rId136"/>
-    <hyperlink ref="B151" r:id="rId137"/>
-    <hyperlink ref="B152" r:id="rId138"/>
-    <hyperlink ref="B153" r:id="rId139"/>
-    <hyperlink ref="B154" r:id="rId140"/>
-    <hyperlink ref="B155" r:id="rId141"/>
-    <hyperlink ref="B156" r:id="rId142"/>
-    <hyperlink ref="B157" r:id="rId143"/>
-    <hyperlink ref="B158" r:id="rId144"/>
-    <hyperlink ref="B159" r:id="rId145"/>
-    <hyperlink ref="B160" r:id="rId146"/>
-    <hyperlink ref="B161" r:id="rId147"/>
-    <hyperlink ref="B162" r:id="rId148"/>
-    <hyperlink ref="B163" r:id="rId149"/>
-    <hyperlink ref="B166" r:id="rId150"/>
-    <hyperlink ref="B167" r:id="rId151"/>
-    <hyperlink ref="B168" r:id="rId152"/>
-    <hyperlink ref="B169" r:id="rId153"/>
-    <hyperlink ref="B170" r:id="rId154"/>
-    <hyperlink ref="B171" r:id="rId155"/>
-    <hyperlink ref="B172" r:id="rId156"/>
-    <hyperlink ref="B173" r:id="rId157"/>
-    <hyperlink ref="B174" r:id="rId158"/>
-    <hyperlink ref="B177" r:id="rId159"/>
-    <hyperlink ref="B178" r:id="rId160"/>
-    <hyperlink ref="B179" r:id="rId161"/>
-    <hyperlink ref="B180" r:id="rId162"/>
-    <hyperlink ref="B181" r:id="rId163"/>
-    <hyperlink ref="B182" r:id="rId164"/>
-    <hyperlink ref="B183" r:id="rId165"/>
-    <hyperlink ref="B184" r:id="rId166"/>
-    <hyperlink ref="B185" r:id="rId167"/>
-    <hyperlink ref="B186" r:id="rId168"/>
-    <hyperlink ref="B187" r:id="rId169"/>
-    <hyperlink ref="B188" r:id="rId170"/>
-    <hyperlink ref="B189" r:id="rId171"/>
-    <hyperlink ref="B190" r:id="rId172"/>
-    <hyperlink ref="B191" r:id="rId173"/>
-    <hyperlink ref="B192" r:id="rId174"/>
-    <hyperlink ref="B193" r:id="rId175"/>
-    <hyperlink ref="B194" r:id="rId176"/>
-    <hyperlink ref="B195" r:id="rId177"/>
-    <hyperlink ref="B196" r:id="rId178"/>
-    <hyperlink ref="B197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
-    <hyperlink ref="B198" r:id="rId180"/>
-    <hyperlink ref="B199" r:id="rId181"/>
-    <hyperlink ref="B200" r:id="rId182"/>
-    <hyperlink ref="B201" r:id="rId183"/>
-    <hyperlink ref="B202" r:id="rId184"/>
-    <hyperlink ref="B203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
-    <hyperlink ref="B204" r:id="rId186"/>
-    <hyperlink ref="B205" r:id="rId187"/>
-    <hyperlink ref="B206" r:id="rId188"/>
-    <hyperlink ref="B207" r:id="rId189"/>
-    <hyperlink ref="B208" r:id="rId190"/>
-    <hyperlink ref="B209" r:id="rId191"/>
-    <hyperlink ref="B210" r:id="rId192"/>
-    <hyperlink ref="B211" r:id="rId193"/>
-    <hyperlink ref="B214" r:id="rId194"/>
-    <hyperlink ref="B215" r:id="rId195"/>
-    <hyperlink ref="B216" r:id="rId196"/>
-    <hyperlink ref="B217" r:id="rId197"/>
-    <hyperlink ref="B218" r:id="rId198"/>
-    <hyperlink ref="B219" r:id="rId199"/>
-    <hyperlink ref="B220" r:id="rId200"/>
-    <hyperlink ref="B221" r:id="rId201"/>
-    <hyperlink ref="B222" r:id="rId202"/>
-    <hyperlink ref="B223" r:id="rId203"/>
-    <hyperlink ref="B224" r:id="rId204"/>
-    <hyperlink ref="B225" r:id="rId205"/>
-    <hyperlink ref="B226" r:id="rId206"/>
-    <hyperlink ref="B227" r:id="rId207"/>
-    <hyperlink ref="B228" r:id="rId208"/>
-    <hyperlink ref="B229" r:id="rId209"/>
-    <hyperlink ref="B230" r:id="rId210"/>
-    <hyperlink ref="B231" r:id="rId211"/>
-    <hyperlink ref="B232" r:id="rId212"/>
-    <hyperlink ref="B233" r:id="rId213"/>
-    <hyperlink ref="B234" r:id="rId214"/>
-    <hyperlink ref="B235" r:id="rId215"/>
-    <hyperlink ref="B238" r:id="rId216"/>
-    <hyperlink ref="B239" r:id="rId217"/>
-    <hyperlink ref="B240" r:id="rId218"/>
-    <hyperlink ref="B241" r:id="rId219"/>
-    <hyperlink ref="B242" r:id="rId220"/>
-    <hyperlink ref="B243" r:id="rId221"/>
-    <hyperlink ref="B244" r:id="rId222"/>
-    <hyperlink ref="B245" r:id="rId223"/>
-    <hyperlink ref="B246" r:id="rId224"/>
-    <hyperlink ref="B247" r:id="rId225"/>
-    <hyperlink ref="B248" r:id="rId226"/>
-    <hyperlink ref="B249" r:id="rId227"/>
-    <hyperlink ref="B250" r:id="rId228"/>
-    <hyperlink ref="B251" r:id="rId229"/>
-    <hyperlink ref="B252" r:id="rId230"/>
-    <hyperlink ref="B253" r:id="rId231"/>
-    <hyperlink ref="B254" r:id="rId232"/>
-    <hyperlink ref="B255" r:id="rId233"/>
-    <hyperlink ref="B256" r:id="rId234"/>
-    <hyperlink ref="B257" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B258" r:id="rId236"/>
-    <hyperlink ref="B259" r:id="rId237"/>
-    <hyperlink ref="B260" r:id="rId238"/>
-    <hyperlink ref="B261" r:id="rId239"/>
-    <hyperlink ref="B262" r:id="rId240"/>
-    <hyperlink ref="B263" r:id="rId241"/>
-    <hyperlink ref="B264" r:id="rId242"/>
-    <hyperlink ref="B265" r:id="rId243"/>
-    <hyperlink ref="B266" r:id="rId244"/>
-    <hyperlink ref="B267" r:id="rId245"/>
-    <hyperlink ref="B268" r:id="rId246"/>
-    <hyperlink ref="B269" r:id="rId247"/>
-    <hyperlink ref="B270" r:id="rId248"/>
-    <hyperlink ref="B271" r:id="rId249"/>
-    <hyperlink ref="B272" r:id="rId250"/>
-    <hyperlink ref="B275" r:id="rId251"/>
-    <hyperlink ref="B276" r:id="rId252"/>
-    <hyperlink ref="B277" r:id="rId253"/>
-    <hyperlink ref="B278" r:id="rId254"/>
-    <hyperlink ref="B279" r:id="rId255"/>
-    <hyperlink ref="B280" r:id="rId256"/>
-    <hyperlink ref="B281" r:id="rId257"/>
-    <hyperlink ref="B282" r:id="rId258"/>
-    <hyperlink ref="B283" r:id="rId259"/>
-    <hyperlink ref="B284" r:id="rId260"/>
-    <hyperlink ref="B285" r:id="rId261"/>
-    <hyperlink ref="B286" r:id="rId262"/>
-    <hyperlink ref="B287" r:id="rId263"/>
-    <hyperlink ref="B288" r:id="rId264"/>
-    <hyperlink ref="B289" r:id="rId265"/>
-    <hyperlink ref="B290" r:id="rId266"/>
-    <hyperlink ref="B291" r:id="rId267"/>
-    <hyperlink ref="B292" r:id="rId268"/>
-    <hyperlink ref="B293" r:id="rId269"/>
-    <hyperlink ref="B296" r:id="rId270"/>
-    <hyperlink ref="B297" r:id="rId271"/>
-    <hyperlink ref="B298" r:id="rId272"/>
-    <hyperlink ref="B299" r:id="rId273"/>
-    <hyperlink ref="B300" r:id="rId274"/>
-    <hyperlink ref="B301" r:id="rId275"/>
-    <hyperlink ref="B302" r:id="rId276"/>
-    <hyperlink ref="B303" r:id="rId277"/>
-    <hyperlink ref="B304" r:id="rId278"/>
-    <hyperlink ref="B305" r:id="rId279"/>
-    <hyperlink ref="B306" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
-    <hyperlink ref="B307" r:id="rId281"/>
-    <hyperlink ref="B308" r:id="rId282"/>
-    <hyperlink ref="B309" r:id="rId283"/>
-    <hyperlink ref="B310" r:id="rId284"/>
-    <hyperlink ref="B311" r:id="rId285"/>
-    <hyperlink ref="B312" r:id="rId286"/>
-    <hyperlink ref="B313" r:id="rId287"/>
-    <hyperlink ref="B314" r:id="rId288"/>
-    <hyperlink ref="B315" r:id="rId289"/>
-    <hyperlink ref="B316" r:id="rId290"/>
-    <hyperlink ref="B317" r:id="rId291"/>
-    <hyperlink ref="B318" r:id="rId292"/>
-    <hyperlink ref="B319" r:id="rId293"/>
-    <hyperlink ref="B320" r:id="rId294"/>
-    <hyperlink ref="B321" r:id="rId295"/>
-    <hyperlink ref="B322" r:id="rId296"/>
-    <hyperlink ref="B323" r:id="rId297"/>
-    <hyperlink ref="B324" r:id="rId298"/>
-    <hyperlink ref="B325" r:id="rId299"/>
-    <hyperlink ref="B326" r:id="rId300"/>
-    <hyperlink ref="B327" r:id="rId301"/>
-    <hyperlink ref="B328" r:id="rId302"/>
-    <hyperlink ref="B329" r:id="rId303"/>
-    <hyperlink ref="B330" r:id="rId304"/>
-    <hyperlink ref="B331" r:id="rId305"/>
-    <hyperlink ref="B332" r:id="rId306"/>
-    <hyperlink ref="B333" r:id="rId307"/>
-    <hyperlink ref="B336" r:id="rId308"/>
-    <hyperlink ref="B337" r:id="rId309"/>
-    <hyperlink ref="B338" r:id="rId310"/>
-    <hyperlink ref="B339" r:id="rId311"/>
-    <hyperlink ref="B340" r:id="rId312"/>
-    <hyperlink ref="B341" r:id="rId313"/>
-    <hyperlink ref="B342" r:id="rId314"/>
-    <hyperlink ref="B343" r:id="rId315"/>
-    <hyperlink ref="B344" r:id="rId316"/>
-    <hyperlink ref="B345" r:id="rId317"/>
-    <hyperlink ref="B346" r:id="rId318"/>
-    <hyperlink ref="B347" r:id="rId319"/>
-    <hyperlink ref="B348" r:id="rId320"/>
-    <hyperlink ref="B349" r:id="rId321"/>
-    <hyperlink ref="B350" r:id="rId322"/>
-    <hyperlink ref="B351" r:id="rId323"/>
-    <hyperlink ref="B352" r:id="rId324"/>
-    <hyperlink ref="B353" r:id="rId325"/>
-    <hyperlink ref="B357" r:id="rId326"/>
-    <hyperlink ref="B358" r:id="rId327"/>
-    <hyperlink ref="B359" r:id="rId328"/>
-    <hyperlink ref="B360" r:id="rId329"/>
-    <hyperlink ref="B361" r:id="rId330"/>
-    <hyperlink ref="B362" r:id="rId331"/>
-    <hyperlink ref="B363" r:id="rId332"/>
-    <hyperlink ref="B364" r:id="rId333"/>
-    <hyperlink ref="B365" r:id="rId334"/>
-    <hyperlink ref="B366" r:id="rId335"/>
-    <hyperlink ref="B367" r:id="rId336"/>
-    <hyperlink ref="B368" r:id="rId337"/>
-    <hyperlink ref="B369" r:id="rId338"/>
-    <hyperlink ref="B370" r:id="rId339"/>
-    <hyperlink ref="B371" r:id="rId340"/>
-    <hyperlink ref="B372" r:id="rId341"/>
-    <hyperlink ref="B373" r:id="rId342"/>
-    <hyperlink ref="B374" r:id="rId343"/>
-    <hyperlink ref="B375" r:id="rId344"/>
-    <hyperlink ref="B376" r:id="rId345"/>
-    <hyperlink ref="B377" r:id="rId346"/>
-    <hyperlink ref="B378" r:id="rId347"/>
-    <hyperlink ref="B379" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B380" r:id="rId349"/>
-    <hyperlink ref="B381" r:id="rId350"/>
-    <hyperlink ref="B382" r:id="rId351"/>
-    <hyperlink ref="B383" r:id="rId352"/>
-    <hyperlink ref="B384" r:id="rId353"/>
-    <hyperlink ref="B385" r:id="rId354"/>
-    <hyperlink ref="B386" r:id="rId355"/>
-    <hyperlink ref="B387" r:id="rId356"/>
-    <hyperlink ref="B388" r:id="rId357"/>
-    <hyperlink ref="B389" r:id="rId358"/>
-    <hyperlink ref="B390" r:id="rId359"/>
-    <hyperlink ref="B391" r:id="rId360"/>
-    <hyperlink ref="B392" r:id="rId361"/>
-    <hyperlink ref="B393" r:id="rId362"/>
-    <hyperlink ref="B394" r:id="rId363"/>
-    <hyperlink ref="B396" r:id="rId364"/>
-    <hyperlink ref="B395" r:id="rId365"/>
-    <hyperlink ref="B397" r:id="rId366"/>
-    <hyperlink ref="B398" r:id="rId367"/>
-    <hyperlink ref="B399" r:id="rId368"/>
-    <hyperlink ref="B402" r:id="rId369"/>
-    <hyperlink ref="B403" r:id="rId370"/>
-    <hyperlink ref="B404" r:id="rId371"/>
-    <hyperlink ref="B405" r:id="rId372"/>
-    <hyperlink ref="B406" r:id="rId373"/>
-    <hyperlink ref="B407" r:id="rId374"/>
-    <hyperlink ref="B410" r:id="rId375"/>
-    <hyperlink ref="B411" r:id="rId376"/>
-    <hyperlink ref="B412" r:id="rId377"/>
-    <hyperlink ref="B413" r:id="rId378"/>
-    <hyperlink ref="B414" r:id="rId379"/>
-    <hyperlink ref="B415" r:id="rId380"/>
-    <hyperlink ref="B416" r:id="rId381"/>
-    <hyperlink ref="B417" r:id="rId382"/>
-    <hyperlink ref="B418" r:id="rId383"/>
-    <hyperlink ref="B419" r:id="rId384"/>
-    <hyperlink ref="B420" r:id="rId385"/>
-    <hyperlink ref="B421" r:id="rId386"/>
-    <hyperlink ref="B422" r:id="rId387"/>
-    <hyperlink ref="B423" r:id="rId388"/>
-    <hyperlink ref="B424" r:id="rId389"/>
-    <hyperlink ref="B425" r:id="rId390"/>
-    <hyperlink ref="B426" r:id="rId391"/>
-    <hyperlink ref="B427" r:id="rId392"/>
-    <hyperlink ref="B428" r:id="rId393"/>
-    <hyperlink ref="B429" r:id="rId394"/>
-    <hyperlink ref="B430" r:id="rId395"/>
-    <hyperlink ref="B431" r:id="rId396"/>
-    <hyperlink ref="B432" r:id="rId397"/>
-    <hyperlink ref="B433" r:id="rId398"/>
-    <hyperlink ref="B434" r:id="rId399"/>
-    <hyperlink ref="B435" r:id="rId400"/>
-    <hyperlink ref="B436" r:id="rId401"/>
-    <hyperlink ref="B437" r:id="rId402"/>
-    <hyperlink ref="B438" r:id="rId403"/>
-    <hyperlink ref="B439" r:id="rId404"/>
-    <hyperlink ref="B440" r:id="rId405"/>
-    <hyperlink ref="B441" r:id="rId406"/>
-    <hyperlink ref="B442" r:id="rId407"/>
-    <hyperlink ref="B443" r:id="rId408"/>
-    <hyperlink ref="B444" r:id="rId409"/>
-    <hyperlink ref="B445" r:id="rId410"/>
-    <hyperlink ref="B446" r:id="rId411"/>
-    <hyperlink ref="B447" r:id="rId412"/>
-    <hyperlink ref="B448" r:id="rId413"/>
-    <hyperlink ref="B449" r:id="rId414"/>
-    <hyperlink ref="B451" r:id="rId415"/>
-    <hyperlink ref="B450" r:id="rId416"/>
-    <hyperlink ref="B452" r:id="rId417"/>
-    <hyperlink ref="B453" r:id="rId418"/>
-    <hyperlink ref="B454" r:id="rId419"/>
-    <hyperlink ref="B455" r:id="rId420"/>
-    <hyperlink ref="B456" r:id="rId421"/>
-    <hyperlink ref="B457" r:id="rId422"/>
-    <hyperlink ref="B458" r:id="rId423"/>
-    <hyperlink ref="B459" r:id="rId424"/>
-    <hyperlink ref="B460" r:id="rId425"/>
-    <hyperlink ref="B461" r:id="rId426"/>
-    <hyperlink ref="B462" r:id="rId427"/>
-    <hyperlink ref="B469" r:id="rId428"/>
-    <hyperlink ref="B468" r:id="rId429"/>
-    <hyperlink ref="B467" r:id="rId430"/>
-    <hyperlink ref="B466" r:id="rId431"/>
-    <hyperlink ref="B465" r:id="rId432"/>
-    <hyperlink ref="B464" r:id="rId433"/>
-    <hyperlink ref="B463" r:id="rId434"/>
-    <hyperlink ref="B472" r:id="rId435"/>
-    <hyperlink ref="B473" r:id="rId436"/>
-    <hyperlink ref="B474" r:id="rId437"/>
-    <hyperlink ref="B475" r:id="rId438"/>
-    <hyperlink ref="B476" r:id="rId439"/>
-    <hyperlink ref="B477" r:id="rId440"/>
-    <hyperlink ref="B478" r:id="rId441"/>
-    <hyperlink ref="B481" r:id="rId442"/>
-    <hyperlink ref="B479" r:id="rId443"/>
-    <hyperlink ref="B480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B356" r:id="rId445"/>
+    <hyperlink ref="B115" r:id="rId124"/>
+    <hyperlink ref="B142" r:id="rId125"/>
+    <hyperlink ref="B143" r:id="rId126"/>
+    <hyperlink ref="B144" r:id="rId127"/>
+    <hyperlink ref="B145" r:id="rId128"/>
+    <hyperlink ref="B146" r:id="rId129"/>
+    <hyperlink ref="B147" r:id="rId130"/>
+    <hyperlink ref="B148" r:id="rId131"/>
+    <hyperlink ref="B149" r:id="rId132"/>
+    <hyperlink ref="B150" r:id="rId133"/>
+    <hyperlink ref="B151" r:id="rId134"/>
+    <hyperlink ref="B152" r:id="rId135"/>
+    <hyperlink ref="B153" r:id="rId136"/>
+    <hyperlink ref="B154" r:id="rId137"/>
+    <hyperlink ref="B155" r:id="rId138"/>
+    <hyperlink ref="B156" r:id="rId139"/>
+    <hyperlink ref="B157" r:id="rId140"/>
+    <hyperlink ref="B158" r:id="rId141"/>
+    <hyperlink ref="B159" r:id="rId142"/>
+    <hyperlink ref="B160" r:id="rId143"/>
+    <hyperlink ref="B161" r:id="rId144"/>
+    <hyperlink ref="B162" r:id="rId145"/>
+    <hyperlink ref="B163" r:id="rId146"/>
+    <hyperlink ref="B164" r:id="rId147"/>
+    <hyperlink ref="B165" r:id="rId148"/>
+    <hyperlink ref="B166" r:id="rId149"/>
+    <hyperlink ref="B169" r:id="rId150"/>
+    <hyperlink ref="B170" r:id="rId151"/>
+    <hyperlink ref="B171" r:id="rId152"/>
+    <hyperlink ref="B172" r:id="rId153"/>
+    <hyperlink ref="B173" r:id="rId154"/>
+    <hyperlink ref="B174" r:id="rId155"/>
+    <hyperlink ref="B175" r:id="rId156"/>
+    <hyperlink ref="B176" r:id="rId157"/>
+    <hyperlink ref="B177" r:id="rId158"/>
+    <hyperlink ref="B180" r:id="rId159"/>
+    <hyperlink ref="B181" r:id="rId160"/>
+    <hyperlink ref="B182" r:id="rId161"/>
+    <hyperlink ref="B183" r:id="rId162"/>
+    <hyperlink ref="B184" r:id="rId163"/>
+    <hyperlink ref="B185" r:id="rId164"/>
+    <hyperlink ref="B186" r:id="rId165"/>
+    <hyperlink ref="B187" r:id="rId166"/>
+    <hyperlink ref="B188" r:id="rId167"/>
+    <hyperlink ref="B189" r:id="rId168"/>
+    <hyperlink ref="B190" r:id="rId169"/>
+    <hyperlink ref="B191" r:id="rId170"/>
+    <hyperlink ref="B192" r:id="rId171"/>
+    <hyperlink ref="B193" r:id="rId172"/>
+    <hyperlink ref="B194" r:id="rId173"/>
+    <hyperlink ref="B195" r:id="rId174"/>
+    <hyperlink ref="B196" r:id="rId175"/>
+    <hyperlink ref="B197" r:id="rId176"/>
+    <hyperlink ref="B198" r:id="rId177"/>
+    <hyperlink ref="B199" r:id="rId178"/>
+    <hyperlink ref="B200" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
+    <hyperlink ref="B201" r:id="rId180"/>
+    <hyperlink ref="B202" r:id="rId181"/>
+    <hyperlink ref="B203" r:id="rId182"/>
+    <hyperlink ref="B204" r:id="rId183"/>
+    <hyperlink ref="B205" r:id="rId184"/>
+    <hyperlink ref="B206" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
+    <hyperlink ref="B207" r:id="rId186"/>
+    <hyperlink ref="B208" r:id="rId187"/>
+    <hyperlink ref="B209" r:id="rId188"/>
+    <hyperlink ref="B210" r:id="rId189"/>
+    <hyperlink ref="B211" r:id="rId190"/>
+    <hyperlink ref="B212" r:id="rId191"/>
+    <hyperlink ref="B213" r:id="rId192"/>
+    <hyperlink ref="B214" r:id="rId193"/>
+    <hyperlink ref="B217" r:id="rId194"/>
+    <hyperlink ref="B218" r:id="rId195"/>
+    <hyperlink ref="B219" r:id="rId196"/>
+    <hyperlink ref="B220" r:id="rId197"/>
+    <hyperlink ref="B221" r:id="rId198"/>
+    <hyperlink ref="B222" r:id="rId199"/>
+    <hyperlink ref="B223" r:id="rId200"/>
+    <hyperlink ref="B224" r:id="rId201"/>
+    <hyperlink ref="B225" r:id="rId202"/>
+    <hyperlink ref="B226" r:id="rId203"/>
+    <hyperlink ref="B227" r:id="rId204"/>
+    <hyperlink ref="B228" r:id="rId205"/>
+    <hyperlink ref="B229" r:id="rId206"/>
+    <hyperlink ref="B230" r:id="rId207"/>
+    <hyperlink ref="B231" r:id="rId208"/>
+    <hyperlink ref="B232" r:id="rId209"/>
+    <hyperlink ref="B233" r:id="rId210"/>
+    <hyperlink ref="B234" r:id="rId211"/>
+    <hyperlink ref="B235" r:id="rId212"/>
+    <hyperlink ref="B236" r:id="rId213"/>
+    <hyperlink ref="B237" r:id="rId214"/>
+    <hyperlink ref="B238" r:id="rId215"/>
+    <hyperlink ref="B241" r:id="rId216"/>
+    <hyperlink ref="B242" r:id="rId217"/>
+    <hyperlink ref="B243" r:id="rId218"/>
+    <hyperlink ref="B244" r:id="rId219"/>
+    <hyperlink ref="B245" r:id="rId220"/>
+    <hyperlink ref="B246" r:id="rId221"/>
+    <hyperlink ref="B247" r:id="rId222"/>
+    <hyperlink ref="B248" r:id="rId223"/>
+    <hyperlink ref="B249" r:id="rId224"/>
+    <hyperlink ref="B250" r:id="rId225"/>
+    <hyperlink ref="B251" r:id="rId226"/>
+    <hyperlink ref="B252" r:id="rId227"/>
+    <hyperlink ref="B253" r:id="rId228"/>
+    <hyperlink ref="B254" r:id="rId229"/>
+    <hyperlink ref="B255" r:id="rId230"/>
+    <hyperlink ref="B256" r:id="rId231"/>
+    <hyperlink ref="B257" r:id="rId232"/>
+    <hyperlink ref="B258" r:id="rId233"/>
+    <hyperlink ref="B259" r:id="rId234"/>
+    <hyperlink ref="B260" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B261" r:id="rId236"/>
+    <hyperlink ref="B262" r:id="rId237"/>
+    <hyperlink ref="B263" r:id="rId238"/>
+    <hyperlink ref="B264" r:id="rId239"/>
+    <hyperlink ref="B265" r:id="rId240"/>
+    <hyperlink ref="B266" r:id="rId241"/>
+    <hyperlink ref="B267" r:id="rId242"/>
+    <hyperlink ref="B268" r:id="rId243"/>
+    <hyperlink ref="B269" r:id="rId244"/>
+    <hyperlink ref="B270" r:id="rId245"/>
+    <hyperlink ref="B271" r:id="rId246"/>
+    <hyperlink ref="B272" r:id="rId247"/>
+    <hyperlink ref="B273" r:id="rId248"/>
+    <hyperlink ref="B274" r:id="rId249"/>
+    <hyperlink ref="B275" r:id="rId250"/>
+    <hyperlink ref="B278" r:id="rId251"/>
+    <hyperlink ref="B279" r:id="rId252"/>
+    <hyperlink ref="B280" r:id="rId253"/>
+    <hyperlink ref="B281" r:id="rId254"/>
+    <hyperlink ref="B282" r:id="rId255"/>
+    <hyperlink ref="B283" r:id="rId256"/>
+    <hyperlink ref="B284" r:id="rId257"/>
+    <hyperlink ref="B285" r:id="rId258"/>
+    <hyperlink ref="B286" r:id="rId259"/>
+    <hyperlink ref="B287" r:id="rId260"/>
+    <hyperlink ref="B288" r:id="rId261"/>
+    <hyperlink ref="B289" r:id="rId262"/>
+    <hyperlink ref="B290" r:id="rId263"/>
+    <hyperlink ref="B291" r:id="rId264"/>
+    <hyperlink ref="B292" r:id="rId265"/>
+    <hyperlink ref="B293" r:id="rId266"/>
+    <hyperlink ref="B294" r:id="rId267"/>
+    <hyperlink ref="B295" r:id="rId268"/>
+    <hyperlink ref="B296" r:id="rId269"/>
+    <hyperlink ref="B299" r:id="rId270"/>
+    <hyperlink ref="B300" r:id="rId271"/>
+    <hyperlink ref="B301" r:id="rId272"/>
+    <hyperlink ref="B302" r:id="rId273"/>
+    <hyperlink ref="B303" r:id="rId274"/>
+    <hyperlink ref="B304" r:id="rId275"/>
+    <hyperlink ref="B305" r:id="rId276"/>
+    <hyperlink ref="B306" r:id="rId277"/>
+    <hyperlink ref="B307" r:id="rId278"/>
+    <hyperlink ref="B308" r:id="rId279"/>
+    <hyperlink ref="B309" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B310" r:id="rId281"/>
+    <hyperlink ref="B311" r:id="rId282"/>
+    <hyperlink ref="B312" r:id="rId283"/>
+    <hyperlink ref="B313" r:id="rId284"/>
+    <hyperlink ref="B314" r:id="rId285"/>
+    <hyperlink ref="B315" r:id="rId286"/>
+    <hyperlink ref="B316" r:id="rId287"/>
+    <hyperlink ref="B317" r:id="rId288"/>
+    <hyperlink ref="B318" r:id="rId289"/>
+    <hyperlink ref="B319" r:id="rId290"/>
+    <hyperlink ref="B320" r:id="rId291"/>
+    <hyperlink ref="B321" r:id="rId292"/>
+    <hyperlink ref="B322" r:id="rId293"/>
+    <hyperlink ref="B323" r:id="rId294"/>
+    <hyperlink ref="B324" r:id="rId295"/>
+    <hyperlink ref="B325" r:id="rId296"/>
+    <hyperlink ref="B326" r:id="rId297"/>
+    <hyperlink ref="B327" r:id="rId298"/>
+    <hyperlink ref="B328" r:id="rId299"/>
+    <hyperlink ref="B329" r:id="rId300"/>
+    <hyperlink ref="B330" r:id="rId301"/>
+    <hyperlink ref="B331" r:id="rId302"/>
+    <hyperlink ref="B332" r:id="rId303"/>
+    <hyperlink ref="B333" r:id="rId304"/>
+    <hyperlink ref="B334" r:id="rId305"/>
+    <hyperlink ref="B335" r:id="rId306"/>
+    <hyperlink ref="B336" r:id="rId307"/>
+    <hyperlink ref="B339" r:id="rId308"/>
+    <hyperlink ref="B340" r:id="rId309"/>
+    <hyperlink ref="B341" r:id="rId310"/>
+    <hyperlink ref="B342" r:id="rId311"/>
+    <hyperlink ref="B343" r:id="rId312"/>
+    <hyperlink ref="B344" r:id="rId313"/>
+    <hyperlink ref="B345" r:id="rId314"/>
+    <hyperlink ref="B346" r:id="rId315"/>
+    <hyperlink ref="B347" r:id="rId316"/>
+    <hyperlink ref="B348" r:id="rId317"/>
+    <hyperlink ref="B349" r:id="rId318"/>
+    <hyperlink ref="B350" r:id="rId319"/>
+    <hyperlink ref="B351" r:id="rId320"/>
+    <hyperlink ref="B352" r:id="rId321"/>
+    <hyperlink ref="B353" r:id="rId322"/>
+    <hyperlink ref="B354" r:id="rId323"/>
+    <hyperlink ref="B355" r:id="rId324"/>
+    <hyperlink ref="B356" r:id="rId325"/>
+    <hyperlink ref="B360" r:id="rId326"/>
+    <hyperlink ref="B361" r:id="rId327"/>
+    <hyperlink ref="B362" r:id="rId328"/>
+    <hyperlink ref="B363" r:id="rId329"/>
+    <hyperlink ref="B364" r:id="rId330"/>
+    <hyperlink ref="B365" r:id="rId331"/>
+    <hyperlink ref="B366" r:id="rId332"/>
+    <hyperlink ref="B367" r:id="rId333"/>
+    <hyperlink ref="B368" r:id="rId334"/>
+    <hyperlink ref="B369" r:id="rId335"/>
+    <hyperlink ref="B370" r:id="rId336"/>
+    <hyperlink ref="B371" r:id="rId337"/>
+    <hyperlink ref="B372" r:id="rId338"/>
+    <hyperlink ref="B373" r:id="rId339"/>
+    <hyperlink ref="B374" r:id="rId340"/>
+    <hyperlink ref="B375" r:id="rId341"/>
+    <hyperlink ref="B376" r:id="rId342"/>
+    <hyperlink ref="B377" r:id="rId343"/>
+    <hyperlink ref="B378" r:id="rId344"/>
+    <hyperlink ref="B379" r:id="rId345"/>
+    <hyperlink ref="B380" r:id="rId346"/>
+    <hyperlink ref="B381" r:id="rId347"/>
+    <hyperlink ref="B382" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B383" r:id="rId349"/>
+    <hyperlink ref="B384" r:id="rId350"/>
+    <hyperlink ref="B385" r:id="rId351"/>
+    <hyperlink ref="B386" r:id="rId352"/>
+    <hyperlink ref="B387" r:id="rId353"/>
+    <hyperlink ref="B388" r:id="rId354"/>
+    <hyperlink ref="B389" r:id="rId355"/>
+    <hyperlink ref="B390" r:id="rId356"/>
+    <hyperlink ref="B391" r:id="rId357"/>
+    <hyperlink ref="B392" r:id="rId358"/>
+    <hyperlink ref="B393" r:id="rId359"/>
+    <hyperlink ref="B394" r:id="rId360"/>
+    <hyperlink ref="B395" r:id="rId361"/>
+    <hyperlink ref="B396" r:id="rId362"/>
+    <hyperlink ref="B397" r:id="rId363"/>
+    <hyperlink ref="B399" r:id="rId364"/>
+    <hyperlink ref="B398" r:id="rId365"/>
+    <hyperlink ref="B400" r:id="rId366"/>
+    <hyperlink ref="B401" r:id="rId367"/>
+    <hyperlink ref="B402" r:id="rId368"/>
+    <hyperlink ref="B405" r:id="rId369"/>
+    <hyperlink ref="B406" r:id="rId370"/>
+    <hyperlink ref="B407" r:id="rId371"/>
+    <hyperlink ref="B408" r:id="rId372"/>
+    <hyperlink ref="B409" r:id="rId373"/>
+    <hyperlink ref="B410" r:id="rId374"/>
+    <hyperlink ref="B413" r:id="rId375"/>
+    <hyperlink ref="B414" r:id="rId376"/>
+    <hyperlink ref="B415" r:id="rId377"/>
+    <hyperlink ref="B416" r:id="rId378"/>
+    <hyperlink ref="B417" r:id="rId379"/>
+    <hyperlink ref="B418" r:id="rId380"/>
+    <hyperlink ref="B419" r:id="rId381"/>
+    <hyperlink ref="B420" r:id="rId382"/>
+    <hyperlink ref="B421" r:id="rId383"/>
+    <hyperlink ref="B422" r:id="rId384"/>
+    <hyperlink ref="B423" r:id="rId385"/>
+    <hyperlink ref="B424" r:id="rId386"/>
+    <hyperlink ref="B425" r:id="rId387"/>
+    <hyperlink ref="B426" r:id="rId388"/>
+    <hyperlink ref="B427" r:id="rId389"/>
+    <hyperlink ref="B428" r:id="rId390"/>
+    <hyperlink ref="B429" r:id="rId391"/>
+    <hyperlink ref="B430" r:id="rId392"/>
+    <hyperlink ref="B431" r:id="rId393"/>
+    <hyperlink ref="B432" r:id="rId394"/>
+    <hyperlink ref="B433" r:id="rId395"/>
+    <hyperlink ref="B434" r:id="rId396"/>
+    <hyperlink ref="B435" r:id="rId397"/>
+    <hyperlink ref="B436" r:id="rId398"/>
+    <hyperlink ref="B437" r:id="rId399"/>
+    <hyperlink ref="B438" r:id="rId400"/>
+    <hyperlink ref="B439" r:id="rId401"/>
+    <hyperlink ref="B440" r:id="rId402"/>
+    <hyperlink ref="B441" r:id="rId403"/>
+    <hyperlink ref="B442" r:id="rId404"/>
+    <hyperlink ref="B443" r:id="rId405"/>
+    <hyperlink ref="B444" r:id="rId406"/>
+    <hyperlink ref="B445" r:id="rId407"/>
+    <hyperlink ref="B446" r:id="rId408"/>
+    <hyperlink ref="B447" r:id="rId409"/>
+    <hyperlink ref="B448" r:id="rId410"/>
+    <hyperlink ref="B449" r:id="rId411"/>
+    <hyperlink ref="B450" r:id="rId412"/>
+    <hyperlink ref="B451" r:id="rId413"/>
+    <hyperlink ref="B452" r:id="rId414"/>
+    <hyperlink ref="B454" r:id="rId415"/>
+    <hyperlink ref="B453" r:id="rId416"/>
+    <hyperlink ref="B455" r:id="rId417"/>
+    <hyperlink ref="B456" r:id="rId418"/>
+    <hyperlink ref="B457" r:id="rId419"/>
+    <hyperlink ref="B458" r:id="rId420"/>
+    <hyperlink ref="B459" r:id="rId421"/>
+    <hyperlink ref="B460" r:id="rId422"/>
+    <hyperlink ref="B461" r:id="rId423"/>
+    <hyperlink ref="B462" r:id="rId424"/>
+    <hyperlink ref="B463" r:id="rId425"/>
+    <hyperlink ref="B464" r:id="rId426"/>
+    <hyperlink ref="B465" r:id="rId427"/>
+    <hyperlink ref="B472" r:id="rId428"/>
+    <hyperlink ref="B471" r:id="rId429"/>
+    <hyperlink ref="B470" r:id="rId430"/>
+    <hyperlink ref="B469" r:id="rId431"/>
+    <hyperlink ref="B468" r:id="rId432"/>
+    <hyperlink ref="B467" r:id="rId433"/>
+    <hyperlink ref="B466" r:id="rId434"/>
+    <hyperlink ref="B475" r:id="rId435"/>
+    <hyperlink ref="B476" r:id="rId436"/>
+    <hyperlink ref="B477" r:id="rId437"/>
+    <hyperlink ref="B478" r:id="rId438"/>
+    <hyperlink ref="B479" r:id="rId439"/>
+    <hyperlink ref="B480" r:id="rId440"/>
+    <hyperlink ref="B481" r:id="rId441"/>
+    <hyperlink ref="B484" r:id="rId442"/>
+    <hyperlink ref="B482" r:id="rId443"/>
+    <hyperlink ref="B483" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B359" r:id="rId445"/>
+    <hyperlink ref="B109" r:id="rId446"/>
+    <hyperlink ref="B111" r:id="rId447"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId446"/>
-  <legacyDrawing r:id="rId447"/>
+  <pageSetup orientation="portrait" r:id="rId448"/>
+  <legacyDrawing r:id="rId449"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added solution for problem Searching In A Array Where Adjacent Differ by Atmost k
</commit_message>
<xml_diff>
--- a/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="470">
   <si>
     <t>Topic:</t>
   </si>
@@ -1464,13 +1464,19 @@
   </si>
   <si>
     <t>Median of two sorted array</t>
+  </si>
+  <si>
+    <t>Repeating Element</t>
+  </si>
+  <si>
+    <t>Allocate minimum number of pages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1620,6 +1626,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1642,7 +1657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1688,6 +1703,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1995,7 +2013,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2003,10 +2021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C490"/>
+  <dimension ref="A1:C492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3161,7 +3179,7 @@
         <v>96</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C111" s="11" t="s">
         <v>463</v>
@@ -3171,19 +3189,19 @@
       <c r="A112" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B112" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>3</v>
+      <c r="B112" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="C112" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="21">
       <c r="A113" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B113" s="12" t="s">
-        <v>106</v>
+      <c r="B113" s="21" t="s">
+        <v>469</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>3</v>
@@ -3194,7 +3212,7 @@
         <v>96</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>3</v>
@@ -3205,7 +3223,7 @@
         <v>96</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>3</v>
@@ -3216,7 +3234,7 @@
         <v>96</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>3</v>
@@ -3227,7 +3245,7 @@
         <v>96</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>3</v>
@@ -3238,7 +3256,7 @@
         <v>96</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>3</v>
@@ -3249,7 +3267,7 @@
         <v>96</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>3</v>
@@ -3260,7 +3278,7 @@
         <v>96</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>3</v>
@@ -3271,7 +3289,7 @@
         <v>96</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>3</v>
@@ -3282,7 +3300,7 @@
         <v>96</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>3</v>
@@ -3293,7 +3311,7 @@
         <v>96</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>3</v>
@@ -3304,7 +3322,7 @@
         <v>96</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>3</v>
@@ -3315,7 +3333,7 @@
         <v>96</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>3</v>
@@ -3326,7 +3344,7 @@
         <v>96</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>3</v>
@@ -3337,7 +3355,7 @@
         <v>96</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>3</v>
@@ -3348,7 +3366,7 @@
         <v>96</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>3</v>
@@ -3359,7 +3377,7 @@
         <v>96</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>3</v>
@@ -3370,7 +3388,7 @@
         <v>96</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>3</v>
@@ -3381,7 +3399,7 @@
         <v>96</v>
       </c>
       <c r="B131" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>3</v>
@@ -3392,7 +3410,7 @@
         <v>96</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>3</v>
@@ -3403,7 +3421,7 @@
         <v>96</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>3</v>
@@ -3414,7 +3432,7 @@
         <v>96</v>
       </c>
       <c r="B134" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>3</v>
@@ -3425,7 +3443,7 @@
         <v>96</v>
       </c>
       <c r="B135" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>3</v>
@@ -3436,7 +3454,7 @@
         <v>96</v>
       </c>
       <c r="B136" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>3</v>
@@ -3447,7 +3465,7 @@
         <v>96</v>
       </c>
       <c r="B137" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>3</v>
@@ -3458,7 +3476,7 @@
         <v>96</v>
       </c>
       <c r="B138" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>3</v>
@@ -3469,44 +3487,44 @@
         <v>96</v>
       </c>
       <c r="B139" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="21">
+      <c r="A140" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B140" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="21">
+      <c r="A141" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B141" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C139" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="21">
-      <c r="B141" s="5"/>
-      <c r="C141" s="3"/>
-    </row>
-    <row r="142" spans="1:3" ht="21">
-      <c r="A142" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B142" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C142" s="10" t="s">
-        <v>463</v>
+      <c r="C141" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21">
-      <c r="A143" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B143" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C143" s="10" t="s">
-        <v>463</v>
-      </c>
+      <c r="B143" s="5"/>
+      <c r="C143" s="3"/>
     </row>
     <row r="144" spans="1:3" ht="21">
       <c r="A144" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C144" s="10" t="s">
         <v>463</v>
@@ -3517,7 +3535,7 @@
         <v>133</v>
       </c>
       <c r="B145" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C145" s="10" t="s">
         <v>463</v>
@@ -3528,7 +3546,7 @@
         <v>133</v>
       </c>
       <c r="B146" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C146" s="10" t="s">
         <v>463</v>
@@ -3539,29 +3557,29 @@
         <v>133</v>
       </c>
       <c r="B147" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C147" s="10" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="21">
-      <c r="A148" s="6" t="s">
+      <c r="A148" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B148" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C148" s="10" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="21">
-      <c r="A149" s="6" t="s">
+      <c r="A149" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B149" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C149" s="10" t="s">
         <v>463</v>
@@ -3572,7 +3590,7 @@
         <v>133</v>
       </c>
       <c r="B150" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C150" s="10" t="s">
         <v>463</v>
@@ -3583,7 +3601,7 @@
         <v>133</v>
       </c>
       <c r="B151" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C151" s="10" t="s">
         <v>463</v>
@@ -3594,7 +3612,7 @@
         <v>133</v>
       </c>
       <c r="B152" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C152" s="10" t="s">
         <v>463</v>
@@ -3605,7 +3623,7 @@
         <v>133</v>
       </c>
       <c r="B153" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C153" s="10" t="s">
         <v>463</v>
@@ -3615,55 +3633,55 @@
       <c r="A154" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B154" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>3</v>
+      <c r="B154" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C154" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21">
       <c r="A155" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B155" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>3</v>
+      <c r="B155" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C155" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="21">
       <c r="A156" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B156" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="C156" s="10" t="s">
-        <v>463</v>
+      <c r="B156" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="21">
       <c r="A157" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B157" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="C157" s="10" t="s">
-        <v>463</v>
+      <c r="B157" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="21">
       <c r="A158" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B158" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>3</v>
+      <c r="B158" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C158" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21">
@@ -3671,7 +3689,7 @@
         <v>133</v>
       </c>
       <c r="B159" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C159" s="10" t="s">
         <v>463</v>
@@ -3681,11 +3699,11 @@
       <c r="A160" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B160" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="C160" s="10" t="s">
-        <v>463</v>
+      <c r="B160" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="21">
@@ -3693,7 +3711,7 @@
         <v>133</v>
       </c>
       <c r="B161" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C161" s="10" t="s">
         <v>463</v>
@@ -3704,7 +3722,7 @@
         <v>133</v>
       </c>
       <c r="B162" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C162" s="10" t="s">
         <v>463</v>
@@ -3714,22 +3732,22 @@
       <c r="A163" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B163" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>3</v>
+      <c r="B163" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C163" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="21">
       <c r="A164" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B164" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>3</v>
+      <c r="B164" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C164" s="10" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="21">
@@ -3737,7 +3755,7 @@
         <v>133</v>
       </c>
       <c r="B165" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>3</v>
@@ -3748,7 +3766,7 @@
         <v>133</v>
       </c>
       <c r="B166" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>3</v>
@@ -3758,8 +3776,8 @@
       <c r="A167" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B167" s="13" t="s">
-        <v>159</v>
+      <c r="B167" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>3</v>
@@ -3769,8 +3787,8 @@
       <c r="A168" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B168" s="13" t="s">
-        <v>160</v>
+      <c r="B168" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>3</v>
@@ -3780,8 +3798,8 @@
       <c r="A169" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B169" s="12" t="s">
-        <v>161</v>
+      <c r="B169" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="C169" s="3" t="s">
         <v>3</v>
@@ -3791,8 +3809,8 @@
       <c r="A170" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B170" s="12" t="s">
-        <v>162</v>
+      <c r="B170" s="13" t="s">
+        <v>160</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>3</v>
@@ -3803,7 +3821,7 @@
         <v>133</v>
       </c>
       <c r="B171" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C171" s="3" t="s">
         <v>3</v>
@@ -3814,7 +3832,7 @@
         <v>133</v>
       </c>
       <c r="B172" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>3</v>
@@ -3825,7 +3843,7 @@
         <v>133</v>
       </c>
       <c r="B173" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>3</v>
@@ -3836,7 +3854,7 @@
         <v>133</v>
       </c>
       <c r="B174" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>3</v>
@@ -3847,7 +3865,7 @@
         <v>133</v>
       </c>
       <c r="B175" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>3</v>
@@ -3858,7 +3876,7 @@
         <v>133</v>
       </c>
       <c r="B176" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>3</v>
@@ -3869,44 +3887,44 @@
         <v>133</v>
       </c>
       <c r="B177" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="21">
+      <c r="A178" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B178" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="21">
+      <c r="A179" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B179" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C177" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="21">
-      <c r="B179" s="5"/>
-      <c r="C179" s="3"/>
-    </row>
-    <row r="180" spans="1:3" ht="21">
-      <c r="A180" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B180" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C180" s="3" t="s">
+      <c r="C179" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
-      <c r="A181" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B181" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B181" s="5"/>
+      <c r="C181" s="3"/>
     </row>
     <row r="182" spans="1:3" ht="21">
       <c r="A182" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B182" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C182" s="3" t="s">
         <v>3</v>
@@ -3917,7 +3935,7 @@
         <v>170</v>
       </c>
       <c r="B183" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>3</v>
@@ -3928,7 +3946,7 @@
         <v>170</v>
       </c>
       <c r="B184" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>3</v>
@@ -3939,7 +3957,7 @@
         <v>170</v>
       </c>
       <c r="B185" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>3</v>
@@ -3950,7 +3968,7 @@
         <v>170</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>3</v>
@@ -3961,7 +3979,7 @@
         <v>170</v>
       </c>
       <c r="B187" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>3</v>
@@ -3972,7 +3990,7 @@
         <v>170</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>3</v>
@@ -3983,7 +4001,7 @@
         <v>170</v>
       </c>
       <c r="B189" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>3</v>
@@ -3994,7 +4012,7 @@
         <v>170</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>3</v>
@@ -4005,7 +4023,7 @@
         <v>170</v>
       </c>
       <c r="B191" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>3</v>
@@ -4016,7 +4034,7 @@
         <v>170</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>3</v>
@@ -4027,7 +4045,7 @@
         <v>170</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>3</v>
@@ -4038,7 +4056,7 @@
         <v>170</v>
       </c>
       <c r="B194" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>3</v>
@@ -4049,7 +4067,7 @@
         <v>170</v>
       </c>
       <c r="B195" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>3</v>
@@ -4060,7 +4078,7 @@
         <v>170</v>
       </c>
       <c r="B196" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>3</v>
@@ -4071,7 +4089,7 @@
         <v>170</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>3</v>
@@ -4082,7 +4100,7 @@
         <v>170</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>3</v>
@@ -4093,7 +4111,7 @@
         <v>170</v>
       </c>
       <c r="B199" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>3</v>
@@ -4104,7 +4122,7 @@
         <v>170</v>
       </c>
       <c r="B200" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>3</v>
@@ -4115,7 +4133,7 @@
         <v>170</v>
       </c>
       <c r="B201" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>3</v>
@@ -4126,7 +4144,7 @@
         <v>170</v>
       </c>
       <c r="B202" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C202" s="3" t="s">
         <v>3</v>
@@ -4137,7 +4155,7 @@
         <v>170</v>
       </c>
       <c r="B203" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>3</v>
@@ -4148,7 +4166,7 @@
         <v>170</v>
       </c>
       <c r="B204" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>3</v>
@@ -4159,7 +4177,7 @@
         <v>170</v>
       </c>
       <c r="B205" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>3</v>
@@ -4170,7 +4188,7 @@
         <v>170</v>
       </c>
       <c r="B206" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>3</v>
@@ -4181,7 +4199,7 @@
         <v>170</v>
       </c>
       <c r="B207" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>3</v>
@@ -4192,7 +4210,7 @@
         <v>170</v>
       </c>
       <c r="B208" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>3</v>
@@ -4203,7 +4221,7 @@
         <v>170</v>
       </c>
       <c r="B209" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>3</v>
@@ -4214,7 +4232,7 @@
         <v>170</v>
       </c>
       <c r="B210" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>3</v>
@@ -4225,7 +4243,7 @@
         <v>170</v>
       </c>
       <c r="B211" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>3</v>
@@ -4236,7 +4254,7 @@
         <v>170</v>
       </c>
       <c r="B212" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>3</v>
@@ -4247,7 +4265,7 @@
         <v>170</v>
       </c>
       <c r="B213" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>3</v>
@@ -4258,50 +4276,50 @@
         <v>170</v>
       </c>
       <c r="B214" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="21">
+      <c r="A215" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B215" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="21">
+      <c r="A216" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B216" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="C214" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" ht="21">
-      <c r="A215" s="6"/>
-      <c r="B215" s="13"/>
-      <c r="C215" s="3"/>
-    </row>
-    <row r="216" spans="1:3" ht="21">
-      <c r="A216" s="6"/>
-      <c r="B216" s="13"/>
-      <c r="C216" s="3"/>
+      <c r="C216" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="217" spans="1:3" ht="21">
-      <c r="A217" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B217" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="C217" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A217" s="6"/>
+      <c r="B217" s="13"/>
+      <c r="C217" s="3"/>
     </row>
     <row r="218" spans="1:3" ht="21">
-      <c r="A218" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B218" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A218" s="6"/>
+      <c r="B218" s="13"/>
+      <c r="C218" s="3"/>
     </row>
     <row r="219" spans="1:3" ht="21">
       <c r="A219" s="4" t="s">
         <v>206</v>
       </c>
       <c r="B219" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>3</v>
@@ -4312,7 +4330,7 @@
         <v>206</v>
       </c>
       <c r="B220" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C220" s="3" t="s">
         <v>3</v>
@@ -4323,7 +4341,7 @@
         <v>206</v>
       </c>
       <c r="B221" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>3</v>
@@ -4334,7 +4352,7 @@
         <v>206</v>
       </c>
       <c r="B222" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>3</v>
@@ -4344,8 +4362,8 @@
       <c r="A223" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B223" s="16" t="s">
-        <v>213</v>
+      <c r="B223" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>3</v>
@@ -4356,7 +4374,7 @@
         <v>206</v>
       </c>
       <c r="B224" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>3</v>
@@ -4366,8 +4384,8 @@
       <c r="A225" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B225" s="12" t="s">
-        <v>215</v>
+      <c r="B225" s="16" t="s">
+        <v>213</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>3</v>
@@ -4378,7 +4396,7 @@
         <v>206</v>
       </c>
       <c r="B226" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>3</v>
@@ -4389,7 +4407,7 @@
         <v>206</v>
       </c>
       <c r="B227" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>3</v>
@@ -4400,7 +4418,7 @@
         <v>206</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C228" s="3" t="s">
         <v>3</v>
@@ -4411,7 +4429,7 @@
         <v>206</v>
       </c>
       <c r="B229" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>3</v>
@@ -4422,7 +4440,7 @@
         <v>206</v>
       </c>
       <c r="B230" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>3</v>
@@ -4433,7 +4451,7 @@
         <v>206</v>
       </c>
       <c r="B231" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>3</v>
@@ -4444,7 +4462,7 @@
         <v>206</v>
       </c>
       <c r="B232" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>3</v>
@@ -4455,7 +4473,7 @@
         <v>206</v>
       </c>
       <c r="B233" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>3</v>
@@ -4466,7 +4484,7 @@
         <v>206</v>
       </c>
       <c r="B234" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>3</v>
@@ -4477,7 +4495,7 @@
         <v>206</v>
       </c>
       <c r="B235" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>3</v>
@@ -4488,7 +4506,7 @@
         <v>206</v>
       </c>
       <c r="B236" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>3</v>
@@ -4499,7 +4517,7 @@
         <v>206</v>
       </c>
       <c r="B237" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>3</v>
@@ -4510,48 +4528,48 @@
         <v>206</v>
       </c>
       <c r="B238" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="21">
+      <c r="A239" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B239" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="21">
+      <c r="A240" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B240" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="C238" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="21">
-      <c r="B239" s="13"/>
-      <c r="C239" s="3"/>
-    </row>
-    <row r="240" spans="1:3" ht="21">
-      <c r="B240" s="13"/>
-      <c r="C240" s="3"/>
+      <c r="C240" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="241" spans="1:3" ht="21">
-      <c r="A241" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B241" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C241" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B241" s="13"/>
+      <c r="C241" s="3"/>
     </row>
     <row r="242" spans="1:3" ht="21">
-      <c r="A242" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B242" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="C242" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B242" s="13"/>
+      <c r="C242" s="3"/>
     </row>
     <row r="243" spans="1:3" ht="21">
       <c r="A243" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B243" s="12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>3</v>
@@ -4562,7 +4580,7 @@
         <v>229</v>
       </c>
       <c r="B244" s="12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>3</v>
@@ -4573,7 +4591,7 @@
         <v>229</v>
       </c>
       <c r="B245" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>3</v>
@@ -4584,7 +4602,7 @@
         <v>229</v>
       </c>
       <c r="B246" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>3</v>
@@ -4595,7 +4613,7 @@
         <v>229</v>
       </c>
       <c r="B247" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>3</v>
@@ -4606,7 +4624,7 @@
         <v>229</v>
       </c>
       <c r="B248" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>3</v>
@@ -4617,7 +4635,7 @@
         <v>229</v>
       </c>
       <c r="B249" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>3</v>
@@ -4628,7 +4646,7 @@
         <v>229</v>
       </c>
       <c r="B250" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C250" s="3" t="s">
         <v>3</v>
@@ -4639,7 +4657,7 @@
         <v>229</v>
       </c>
       <c r="B251" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C251" s="3" t="s">
         <v>3</v>
@@ -4650,7 +4668,7 @@
         <v>229</v>
       </c>
       <c r="B252" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C252" s="3" t="s">
         <v>3</v>
@@ -4661,7 +4679,7 @@
         <v>229</v>
       </c>
       <c r="B253" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C253" s="3" t="s">
         <v>3</v>
@@ -4672,7 +4690,7 @@
         <v>229</v>
       </c>
       <c r="B254" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>3</v>
@@ -4683,7 +4701,7 @@
         <v>229</v>
       </c>
       <c r="B255" s="12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>3</v>
@@ -4694,7 +4712,7 @@
         <v>229</v>
       </c>
       <c r="B256" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>3</v>
@@ -4705,7 +4723,7 @@
         <v>229</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>3</v>
@@ -4716,7 +4734,7 @@
         <v>229</v>
       </c>
       <c r="B258" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>3</v>
@@ -4727,7 +4745,7 @@
         <v>229</v>
       </c>
       <c r="B259" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>3</v>
@@ -4738,7 +4756,7 @@
         <v>229</v>
       </c>
       <c r="B260" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>3</v>
@@ -4749,7 +4767,7 @@
         <v>229</v>
       </c>
       <c r="B261" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>3</v>
@@ -4760,7 +4778,7 @@
         <v>229</v>
       </c>
       <c r="B262" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C262" s="3" t="s">
         <v>3</v>
@@ -4771,7 +4789,7 @@
         <v>229</v>
       </c>
       <c r="B263" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>3</v>
@@ -4782,7 +4800,7 @@
         <v>229</v>
       </c>
       <c r="B264" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C264" s="3" t="s">
         <v>3</v>
@@ -4793,7 +4811,7 @@
         <v>229</v>
       </c>
       <c r="B265" s="12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>3</v>
@@ -4804,7 +4822,7 @@
         <v>229</v>
       </c>
       <c r="B266" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>3</v>
@@ -4815,7 +4833,7 @@
         <v>229</v>
       </c>
       <c r="B267" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>3</v>
@@ -4826,7 +4844,7 @@
         <v>229</v>
       </c>
       <c r="B268" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C268" s="3" t="s">
         <v>3</v>
@@ -4837,7 +4855,7 @@
         <v>229</v>
       </c>
       <c r="B269" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C269" s="3" t="s">
         <v>3</v>
@@ -4848,7 +4866,7 @@
         <v>229</v>
       </c>
       <c r="B270" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C270" s="3" t="s">
         <v>3</v>
@@ -4859,7 +4877,7 @@
         <v>229</v>
       </c>
       <c r="B271" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C271" s="3" t="s">
         <v>3</v>
@@ -4870,7 +4888,7 @@
         <v>229</v>
       </c>
       <c r="B272" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>3</v>
@@ -4881,7 +4899,7 @@
         <v>229</v>
       </c>
       <c r="B273" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>3</v>
@@ -4892,7 +4910,7 @@
         <v>229</v>
       </c>
       <c r="B274" s="12" t="s">
-        <v>86</v>
+        <v>261</v>
       </c>
       <c r="C274" s="3" t="s">
         <v>3</v>
@@ -4903,48 +4921,48 @@
         <v>229</v>
       </c>
       <c r="B275" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C275" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="21">
+      <c r="A276" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B276" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C276" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" ht="21">
+      <c r="A277" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B277" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="C275" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" ht="21">
-      <c r="B276" s="13"/>
-      <c r="C276" s="3"/>
-    </row>
-    <row r="277" spans="1:3" ht="21">
-      <c r="B277" s="13"/>
-      <c r="C277" s="3"/>
+      <c r="C277" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="278" spans="1:3" ht="21">
-      <c r="A278" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B278" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C278" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B278" s="13"/>
+      <c r="C278" s="3"/>
     </row>
     <row r="279" spans="1:3" ht="21">
-      <c r="A279" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B279" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="C279" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B279" s="13"/>
+      <c r="C279" s="3"/>
     </row>
     <row r="280" spans="1:3" ht="21">
       <c r="A280" s="4" t="s">
         <v>264</v>
       </c>
       <c r="B280" s="12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C280" s="3" t="s">
         <v>3</v>
@@ -4955,7 +4973,7 @@
         <v>264</v>
       </c>
       <c r="B281" s="12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C281" s="3" t="s">
         <v>3</v>
@@ -4966,7 +4984,7 @@
         <v>264</v>
       </c>
       <c r="B282" s="12" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>3</v>
@@ -4977,7 +4995,7 @@
         <v>264</v>
       </c>
       <c r="B283" s="12" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>3</v>
@@ -4988,7 +5006,7 @@
         <v>264</v>
       </c>
       <c r="B284" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>3</v>
@@ -4999,7 +5017,7 @@
         <v>264</v>
       </c>
       <c r="B285" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C285" s="3" t="s">
         <v>3</v>
@@ -5010,7 +5028,7 @@
         <v>264</v>
       </c>
       <c r="B286" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C286" s="3" t="s">
         <v>3</v>
@@ -5021,7 +5039,7 @@
         <v>264</v>
       </c>
       <c r="B287" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C287" s="3" t="s">
         <v>3</v>
@@ -5032,7 +5050,7 @@
         <v>264</v>
       </c>
       <c r="B288" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>3</v>
@@ -5043,7 +5061,7 @@
         <v>264</v>
       </c>
       <c r="B289" s="12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C289" s="3" t="s">
         <v>3</v>
@@ -5054,7 +5072,7 @@
         <v>264</v>
       </c>
       <c r="B290" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C290" s="3" t="s">
         <v>3</v>
@@ -5065,7 +5083,7 @@
         <v>264</v>
       </c>
       <c r="B291" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>3</v>
@@ -5076,7 +5094,7 @@
         <v>264</v>
       </c>
       <c r="B292" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>3</v>
@@ -5087,7 +5105,7 @@
         <v>264</v>
       </c>
       <c r="B293" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C293" s="3" t="s">
         <v>3</v>
@@ -5098,7 +5116,7 @@
         <v>264</v>
       </c>
       <c r="B294" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C294" s="3" t="s">
         <v>3</v>
@@ -5109,7 +5127,7 @@
         <v>264</v>
       </c>
       <c r="B295" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C295" s="3" t="s">
         <v>3</v>
@@ -5120,48 +5138,48 @@
         <v>264</v>
       </c>
       <c r="B296" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" ht="21">
+      <c r="A297" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B297" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C297" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" ht="21">
+      <c r="A298" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B298" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="C296" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" ht="21">
-      <c r="B297" s="13"/>
-      <c r="C297" s="3"/>
-    </row>
-    <row r="298" spans="1:3" ht="21">
-      <c r="B298" s="13"/>
-      <c r="C298" s="3"/>
+      <c r="C298" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="299" spans="1:3" ht="21">
-      <c r="A299" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B299" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="C299" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B299" s="13"/>
+      <c r="C299" s="3"/>
     </row>
     <row r="300" spans="1:3" ht="21">
-      <c r="A300" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B300" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="C300" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B300" s="13"/>
+      <c r="C300" s="3"/>
     </row>
     <row r="301" spans="1:3" ht="21">
       <c r="A301" s="4" t="s">
         <v>284</v>
       </c>
       <c r="B301" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C301" s="3" t="s">
         <v>3</v>
@@ -5172,7 +5190,7 @@
         <v>284</v>
       </c>
       <c r="B302" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C302" s="3" t="s">
         <v>3</v>
@@ -5183,7 +5201,7 @@
         <v>284</v>
       </c>
       <c r="B303" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C303" s="3" t="s">
         <v>3</v>
@@ -5194,7 +5212,7 @@
         <v>284</v>
       </c>
       <c r="B304" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C304" s="3" t="s">
         <v>3</v>
@@ -5205,7 +5223,7 @@
         <v>284</v>
       </c>
       <c r="B305" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C305" s="3" t="s">
         <v>3</v>
@@ -5216,7 +5234,7 @@
         <v>284</v>
       </c>
       <c r="B306" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C306" s="3" t="s">
         <v>3</v>
@@ -5227,7 +5245,7 @@
         <v>284</v>
       </c>
       <c r="B307" s="12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C307" s="3" t="s">
         <v>3</v>
@@ -5238,7 +5256,7 @@
         <v>284</v>
       </c>
       <c r="B308" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C308" s="3" t="s">
         <v>3</v>
@@ -5249,7 +5267,7 @@
         <v>284</v>
       </c>
       <c r="B309" s="12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C309" s="3" t="s">
         <v>3</v>
@@ -5260,7 +5278,7 @@
         <v>284</v>
       </c>
       <c r="B310" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C310" s="3" t="s">
         <v>3</v>
@@ -5271,7 +5289,7 @@
         <v>284</v>
       </c>
       <c r="B311" s="12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C311" s="3" t="s">
         <v>3</v>
@@ -5281,8 +5299,8 @@
       <c r="A312" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B312" s="16" t="s">
-        <v>298</v>
+      <c r="B312" s="12" t="s">
+        <v>296</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>3</v>
@@ -5293,7 +5311,7 @@
         <v>284</v>
       </c>
       <c r="B313" s="12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C313" s="3" t="s">
         <v>3</v>
@@ -5303,8 +5321,8 @@
       <c r="A314" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B314" s="12" t="s">
-        <v>300</v>
+      <c r="B314" s="16" t="s">
+        <v>298</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>3</v>
@@ -5315,7 +5333,7 @@
         <v>284</v>
       </c>
       <c r="B315" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>3</v>
@@ -5326,7 +5344,7 @@
         <v>284</v>
       </c>
       <c r="B316" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C316" s="3" t="s">
         <v>3</v>
@@ -5337,7 +5355,7 @@
         <v>284</v>
       </c>
       <c r="B317" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>3</v>
@@ -5348,7 +5366,7 @@
         <v>284</v>
       </c>
       <c r="B318" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>3</v>
@@ -5359,7 +5377,7 @@
         <v>284</v>
       </c>
       <c r="B319" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>3</v>
@@ -5370,7 +5388,7 @@
         <v>284</v>
       </c>
       <c r="B320" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C320" s="3" t="s">
         <v>3</v>
@@ -5381,7 +5399,7 @@
         <v>284</v>
       </c>
       <c r="B321" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C321" s="3" t="s">
         <v>3</v>
@@ -5392,7 +5410,7 @@
         <v>284</v>
       </c>
       <c r="B322" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C322" s="3" t="s">
         <v>3</v>
@@ -5403,7 +5421,7 @@
         <v>284</v>
       </c>
       <c r="B323" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C323" s="3" t="s">
         <v>3</v>
@@ -5414,7 +5432,7 @@
         <v>284</v>
       </c>
       <c r="B324" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C324" s="3" t="s">
         <v>3</v>
@@ -5425,7 +5443,7 @@
         <v>284</v>
       </c>
       <c r="B325" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C325" s="3" t="s">
         <v>3</v>
@@ -5436,7 +5454,7 @@
         <v>284</v>
       </c>
       <c r="B326" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>3</v>
@@ -5447,7 +5465,7 @@
         <v>284</v>
       </c>
       <c r="B327" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C327" s="3" t="s">
         <v>3</v>
@@ -5458,7 +5476,7 @@
         <v>284</v>
       </c>
       <c r="B328" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>3</v>
@@ -5469,7 +5487,7 @@
         <v>284</v>
       </c>
       <c r="B329" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C329" s="3" t="s">
         <v>3</v>
@@ -5480,7 +5498,7 @@
         <v>284</v>
       </c>
       <c r="B330" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C330" s="3" t="s">
         <v>3</v>
@@ -5491,7 +5509,7 @@
         <v>284</v>
       </c>
       <c r="B331" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C331" s="3" t="s">
         <v>3</v>
@@ -5502,7 +5520,7 @@
         <v>284</v>
       </c>
       <c r="B332" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>3</v>
@@ -5513,7 +5531,7 @@
         <v>284</v>
       </c>
       <c r="B333" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C333" s="3" t="s">
         <v>3</v>
@@ -5524,7 +5542,7 @@
         <v>284</v>
       </c>
       <c r="B334" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C334" s="3" t="s">
         <v>3</v>
@@ -5535,7 +5553,7 @@
         <v>284</v>
       </c>
       <c r="B335" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C335" s="3" t="s">
         <v>3</v>
@@ -5546,48 +5564,48 @@
         <v>284</v>
       </c>
       <c r="B336" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="C336" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" ht="21">
+      <c r="A337" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B337" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C337" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" ht="21">
+      <c r="A338" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B338" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="C336" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="337" spans="1:3" ht="21">
-      <c r="B337" s="13"/>
-      <c r="C337" s="3"/>
-    </row>
-    <row r="338" spans="1:3" ht="21">
-      <c r="B338" s="13"/>
-      <c r="C338" s="3"/>
+      <c r="C338" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="339" spans="1:3" ht="21">
-      <c r="A339" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="B339" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="C339" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B339" s="13"/>
+      <c r="C339" s="3"/>
     </row>
     <row r="340" spans="1:3" ht="21">
-      <c r="A340" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="B340" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="C340" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B340" s="13"/>
+      <c r="C340" s="3"/>
     </row>
     <row r="341" spans="1:3" ht="21">
       <c r="A341" s="6" t="s">
         <v>323</v>
       </c>
       <c r="B341" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C341" s="3" t="s">
         <v>3</v>
@@ -5598,7 +5616,7 @@
         <v>323</v>
       </c>
       <c r="B342" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C342" s="3" t="s">
         <v>3</v>
@@ -5609,7 +5627,7 @@
         <v>323</v>
       </c>
       <c r="B343" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C343" s="3" t="s">
         <v>3</v>
@@ -5620,7 +5638,7 @@
         <v>323</v>
       </c>
       <c r="B344" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>3</v>
@@ -5631,7 +5649,7 @@
         <v>323</v>
       </c>
       <c r="B345" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C345" s="3" t="s">
         <v>3</v>
@@ -5642,7 +5660,7 @@
         <v>323</v>
       </c>
       <c r="B346" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C346" s="3" t="s">
         <v>3</v>
@@ -5652,8 +5670,8 @@
       <c r="A347" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B347" s="16" t="s">
-        <v>332</v>
+      <c r="B347" s="12" t="s">
+        <v>330</v>
       </c>
       <c r="C347" s="3" t="s">
         <v>3</v>
@@ -5664,7 +5682,7 @@
         <v>323</v>
       </c>
       <c r="B348" s="12" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C348" s="3" t="s">
         <v>3</v>
@@ -5674,8 +5692,8 @@
       <c r="A349" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B349" s="12" t="s">
-        <v>334</v>
+      <c r="B349" s="16" t="s">
+        <v>332</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>3</v>
@@ -5686,7 +5704,7 @@
         <v>323</v>
       </c>
       <c r="B350" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C350" s="3" t="s">
         <v>3</v>
@@ -5697,7 +5715,7 @@
         <v>323</v>
       </c>
       <c r="B351" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C351" s="3" t="s">
         <v>3</v>
@@ -5708,7 +5726,7 @@
         <v>323</v>
       </c>
       <c r="B352" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C352" s="3" t="s">
         <v>3</v>
@@ -5719,7 +5737,7 @@
         <v>323</v>
       </c>
       <c r="B353" s="12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C353" s="3" t="s">
         <v>3</v>
@@ -5730,7 +5748,7 @@
         <v>323</v>
       </c>
       <c r="B354" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C354" s="3" t="s">
         <v>3</v>
@@ -5741,7 +5759,7 @@
         <v>323</v>
       </c>
       <c r="B355" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C355" s="3" t="s">
         <v>3</v>
@@ -5752,48 +5770,48 @@
         <v>323</v>
       </c>
       <c r="B356" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="C356" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" ht="21">
+      <c r="A357" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B357" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="C357" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" ht="21">
+      <c r="A358" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B358" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="C356" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="357" spans="1:3" ht="21">
-      <c r="B357" s="13"/>
-      <c r="C357" s="3"/>
-    </row>
-    <row r="358" spans="1:3" ht="21">
-      <c r="B358" s="13"/>
-      <c r="C358" s="3"/>
+      <c r="C358" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="359" spans="1:3" ht="21">
-      <c r="A359" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="B359" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="C359" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B359" s="13"/>
+      <c r="C359" s="3"/>
     </row>
     <row r="360" spans="1:3" ht="21">
-      <c r="A360" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="B360" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="C360" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B360" s="13"/>
+      <c r="C360" s="3"/>
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="6" t="s">
         <v>342</v>
       </c>
       <c r="B361" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C361" s="3" t="s">
         <v>3</v>
@@ -5804,7 +5822,7 @@
         <v>342</v>
       </c>
       <c r="B362" s="12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C362" s="3" t="s">
         <v>3</v>
@@ -5815,7 +5833,7 @@
         <v>342</v>
       </c>
       <c r="B363" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C363" s="3" t="s">
         <v>3</v>
@@ -5826,7 +5844,7 @@
         <v>342</v>
       </c>
       <c r="B364" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C364" s="3" t="s">
         <v>3</v>
@@ -5837,7 +5855,7 @@
         <v>342</v>
       </c>
       <c r="B365" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C365" s="3" t="s">
         <v>3</v>
@@ -5848,7 +5866,7 @@
         <v>342</v>
       </c>
       <c r="B366" s="12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C366" s="3" t="s">
         <v>3</v>
@@ -5859,7 +5877,7 @@
         <v>342</v>
       </c>
       <c r="B367" s="12" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C367" s="3" t="s">
         <v>3</v>
@@ -5870,7 +5888,7 @@
         <v>342</v>
       </c>
       <c r="B368" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C368" s="3" t="s">
         <v>3</v>
@@ -5881,7 +5899,7 @@
         <v>342</v>
       </c>
       <c r="B369" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C369" s="3" t="s">
         <v>3</v>
@@ -5892,7 +5910,7 @@
         <v>342</v>
       </c>
       <c r="B370" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C370" s="3" t="s">
         <v>3</v>
@@ -5903,7 +5921,7 @@
         <v>342</v>
       </c>
       <c r="B371" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C371" s="3" t="s">
         <v>3</v>
@@ -5914,7 +5932,7 @@
         <v>342</v>
       </c>
       <c r="B372" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C372" s="3" t="s">
         <v>3</v>
@@ -5925,7 +5943,7 @@
         <v>342</v>
       </c>
       <c r="B373" s="12" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>3</v>
@@ -5936,7 +5954,7 @@
         <v>342</v>
       </c>
       <c r="B374" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>3</v>
@@ -5947,7 +5965,7 @@
         <v>342</v>
       </c>
       <c r="B375" s="12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>3</v>
@@ -5958,7 +5976,7 @@
         <v>342</v>
       </c>
       <c r="B376" s="12" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>3</v>
@@ -5969,7 +5987,7 @@
         <v>342</v>
       </c>
       <c r="B377" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>3</v>
@@ -5980,7 +5998,7 @@
         <v>342</v>
       </c>
       <c r="B378" s="12" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C378" s="3" t="s">
         <v>3</v>
@@ -5991,7 +6009,7 @@
         <v>342</v>
       </c>
       <c r="B379" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C379" s="3" t="s">
         <v>3</v>
@@ -6002,7 +6020,7 @@
         <v>342</v>
       </c>
       <c r="B380" s="12" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C380" s="3" t="s">
         <v>3</v>
@@ -6013,7 +6031,7 @@
         <v>342</v>
       </c>
       <c r="B381" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C381" s="3" t="s">
         <v>3</v>
@@ -6024,7 +6042,7 @@
         <v>342</v>
       </c>
       <c r="B382" s="12" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C382" s="3" t="s">
         <v>3</v>
@@ -6035,7 +6053,7 @@
         <v>342</v>
       </c>
       <c r="B383" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C383" s="3" t="s">
         <v>3</v>
@@ -6046,7 +6064,7 @@
         <v>342</v>
       </c>
       <c r="B384" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C384" s="3" t="s">
         <v>3</v>
@@ -6057,7 +6075,7 @@
         <v>342</v>
       </c>
       <c r="B385" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C385" s="3" t="s">
         <v>3</v>
@@ -6068,7 +6086,7 @@
         <v>342</v>
       </c>
       <c r="B386" s="12" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C386" s="3" t="s">
         <v>3</v>
@@ -6079,7 +6097,7 @@
         <v>342</v>
       </c>
       <c r="B387" s="12" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C387" s="3" t="s">
         <v>3</v>
@@ -6090,7 +6108,7 @@
         <v>342</v>
       </c>
       <c r="B388" s="12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C388" s="3" t="s">
         <v>3</v>
@@ -6101,7 +6119,7 @@
         <v>342</v>
       </c>
       <c r="B389" s="12" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C389" s="3" t="s">
         <v>3</v>
@@ -6112,7 +6130,7 @@
         <v>342</v>
       </c>
       <c r="B390" s="12" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C390" s="3" t="s">
         <v>3</v>
@@ -6123,7 +6141,7 @@
         <v>342</v>
       </c>
       <c r="B391" s="12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C391" s="3" t="s">
         <v>3</v>
@@ -6134,7 +6152,7 @@
         <v>342</v>
       </c>
       <c r="B392" s="12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C392" s="3" t="s">
         <v>3</v>
@@ -6145,7 +6163,7 @@
         <v>342</v>
       </c>
       <c r="B393" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C393" s="3" t="s">
         <v>3</v>
@@ -6156,7 +6174,7 @@
         <v>342</v>
       </c>
       <c r="B394" s="12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C394" s="3" t="s">
         <v>3</v>
@@ -6167,7 +6185,7 @@
         <v>342</v>
       </c>
       <c r="B395" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C395" s="3" t="s">
         <v>3</v>
@@ -6178,7 +6196,7 @@
         <v>342</v>
       </c>
       <c r="B396" s="12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C396" s="3" t="s">
         <v>3</v>
@@ -6189,7 +6207,7 @@
         <v>342</v>
       </c>
       <c r="B397" s="12" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C397" s="3" t="s">
         <v>3</v>
@@ -6200,7 +6218,7 @@
         <v>342</v>
       </c>
       <c r="B398" s="12" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C398" s="3" t="s">
         <v>3</v>
@@ -6211,7 +6229,7 @@
         <v>342</v>
       </c>
       <c r="B399" s="12" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C399" s="3" t="s">
         <v>3</v>
@@ -6222,7 +6240,7 @@
         <v>342</v>
       </c>
       <c r="B400" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C400" s="3" t="s">
         <v>3</v>
@@ -6233,7 +6251,7 @@
         <v>342</v>
       </c>
       <c r="B401" s="12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C401" s="3" t="s">
         <v>3</v>
@@ -6244,48 +6262,48 @@
         <v>342</v>
       </c>
       <c r="B402" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C402" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" ht="21">
+      <c r="A403" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B403" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="C403" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" ht="21">
+      <c r="A404" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B404" s="12" t="s">
         <v>385</v>
       </c>
-      <c r="C402" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="403" spans="1:3" ht="21">
-      <c r="B403" s="13"/>
-      <c r="C403" s="3"/>
-    </row>
-    <row r="404" spans="1:3" ht="21">
-      <c r="B404" s="13"/>
-      <c r="C404" s="3"/>
+      <c r="C404" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="405" spans="1:3" ht="21">
-      <c r="A405" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B405" s="12" t="s">
-        <v>387</v>
-      </c>
-      <c r="C405" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B405" s="13"/>
+      <c r="C405" s="3"/>
     </row>
     <row r="406" spans="1:3" ht="21">
-      <c r="A406" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B406" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="C406" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B406" s="13"/>
+      <c r="C406" s="3"/>
     </row>
     <row r="407" spans="1:3" ht="21">
       <c r="A407" s="6" t="s">
         <v>386</v>
       </c>
       <c r="B407" s="12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C407" s="3" t="s">
         <v>3</v>
@@ -6296,7 +6314,7 @@
         <v>386</v>
       </c>
       <c r="B408" s="12" t="s">
-        <v>88</v>
+        <v>388</v>
       </c>
       <c r="C408" s="3" t="s">
         <v>3</v>
@@ -6307,7 +6325,7 @@
         <v>386</v>
       </c>
       <c r="B409" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C409" s="3" t="s">
         <v>3</v>
@@ -6318,48 +6336,48 @@
         <v>386</v>
       </c>
       <c r="B410" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C410" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" ht="21">
+      <c r="A411" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B411" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="C411" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" ht="21">
+      <c r="A412" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B412" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="C410" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="411" spans="1:3" ht="21">
-      <c r="B411" s="13"/>
-      <c r="C411" s="3"/>
-    </row>
-    <row r="412" spans="1:3" ht="21">
-      <c r="B412" s="13"/>
-      <c r="C412" s="3"/>
+      <c r="C412" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="413" spans="1:3" ht="21">
-      <c r="A413" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B413" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="C413" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B413" s="13"/>
+      <c r="C413" s="3"/>
     </row>
     <row r="414" spans="1:3" ht="21">
-      <c r="A414" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B414" s="12" t="s">
-        <v>394</v>
-      </c>
-      <c r="C414" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B414" s="13"/>
+      <c r="C414" s="3"/>
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="A415" s="4" t="s">
         <v>392</v>
       </c>
       <c r="B415" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C415" s="3" t="s">
         <v>3</v>
@@ -6370,7 +6388,7 @@
         <v>392</v>
       </c>
       <c r="B416" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C416" s="3" t="s">
         <v>3</v>
@@ -6381,7 +6399,7 @@
         <v>392</v>
       </c>
       <c r="B417" s="12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C417" s="3" t="s">
         <v>3</v>
@@ -6392,7 +6410,7 @@
         <v>392</v>
       </c>
       <c r="B418" s="12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C418" s="3" t="s">
         <v>3</v>
@@ -6403,7 +6421,7 @@
         <v>392</v>
       </c>
       <c r="B419" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C419" s="3" t="s">
         <v>3</v>
@@ -6414,7 +6432,7 @@
         <v>392</v>
       </c>
       <c r="B420" s="12" t="s">
-        <v>272</v>
+        <v>398</v>
       </c>
       <c r="C420" s="3" t="s">
         <v>3</v>
@@ -6425,7 +6443,7 @@
         <v>392</v>
       </c>
       <c r="B421" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C421" s="3" t="s">
         <v>3</v>
@@ -6436,7 +6454,7 @@
         <v>392</v>
       </c>
       <c r="B422" s="12" t="s">
-        <v>401</v>
+        <v>272</v>
       </c>
       <c r="C422" s="3" t="s">
         <v>3</v>
@@ -6447,7 +6465,7 @@
         <v>392</v>
       </c>
       <c r="B423" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C423" s="3" t="s">
         <v>3</v>
@@ -6458,7 +6476,7 @@
         <v>392</v>
       </c>
       <c r="B424" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C424" s="3" t="s">
         <v>3</v>
@@ -6469,7 +6487,7 @@
         <v>392</v>
       </c>
       <c r="B425" s="12" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C425" s="3" t="s">
         <v>3</v>
@@ -6480,7 +6498,7 @@
         <v>392</v>
       </c>
       <c r="B426" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C426" s="3" t="s">
         <v>3</v>
@@ -6491,7 +6509,7 @@
         <v>392</v>
       </c>
       <c r="B427" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C427" s="3" t="s">
         <v>3</v>
@@ -6502,7 +6520,7 @@
         <v>392</v>
       </c>
       <c r="B428" s="12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C428" s="3" t="s">
         <v>3</v>
@@ -6513,7 +6531,7 @@
         <v>392</v>
       </c>
       <c r="B429" s="12" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C429" s="3" t="s">
         <v>3</v>
@@ -6524,7 +6542,7 @@
         <v>392</v>
       </c>
       <c r="B430" s="12" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C430" s="3" t="s">
         <v>3</v>
@@ -6535,7 +6553,7 @@
         <v>392</v>
       </c>
       <c r="B431" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C431" s="3" t="s">
         <v>3</v>
@@ -6546,7 +6564,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C432" s="3" t="s">
         <v>3</v>
@@ -6557,7 +6575,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C433" s="3" t="s">
         <v>3</v>
@@ -6568,7 +6586,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C434" s="3" t="s">
         <v>3</v>
@@ -6579,7 +6597,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C435" s="3" t="s">
         <v>3</v>
@@ -6590,7 +6608,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C436" s="3" t="s">
         <v>3</v>
@@ -6601,7 +6619,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C437" s="3" t="s">
         <v>3</v>
@@ -6612,7 +6630,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C438" s="3" t="s">
         <v>3</v>
@@ -6623,7 +6641,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C439" s="3" t="s">
         <v>3</v>
@@ -6634,7 +6652,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C440" s="3" t="s">
         <v>3</v>
@@ -6645,7 +6663,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="12" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C441" s="3" t="s">
         <v>3</v>
@@ -6656,7 +6674,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C442" s="3" t="s">
         <v>3</v>
@@ -6667,7 +6685,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C443" s="3" t="s">
         <v>3</v>
@@ -6678,7 +6696,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C444" s="3" t="s">
         <v>3</v>
@@ -6689,7 +6707,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C445" s="3" t="s">
         <v>3</v>
@@ -6700,7 +6718,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="12" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C446" s="3" t="s">
         <v>3</v>
@@ -6711,7 +6729,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="12" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C447" s="3" t="s">
         <v>3</v>
@@ -6722,7 +6740,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="12" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C448" s="3" t="s">
         <v>3</v>
@@ -6733,7 +6751,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C449" s="3" t="s">
         <v>3</v>
@@ -6744,7 +6762,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C450" s="3" t="s">
         <v>3</v>
@@ -6755,7 +6773,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C451" s="3" t="s">
         <v>3</v>
@@ -6766,7 +6784,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C452" s="3" t="s">
         <v>3</v>
@@ -6777,7 +6795,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C453" s="3" t="s">
         <v>3</v>
@@ -6788,7 +6806,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="12" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C454" s="3" t="s">
         <v>3</v>
@@ -6799,7 +6817,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="12" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C455" s="3" t="s">
         <v>3</v>
@@ -6810,7 +6828,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="12" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C456" s="3" t="s">
         <v>3</v>
@@ -6821,7 +6839,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C457" s="3" t="s">
         <v>3</v>
@@ -6832,7 +6850,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="12" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C458" s="3" t="s">
         <v>3</v>
@@ -6843,7 +6861,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="12" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C459" s="3" t="s">
         <v>3</v>
@@ -6854,7 +6872,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="12" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C460" s="3" t="s">
         <v>3</v>
@@ -6865,7 +6883,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="12" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C461" s="3" t="s">
         <v>3</v>
@@ -6876,7 +6894,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C462" s="3" t="s">
         <v>3</v>
@@ -6887,7 +6905,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C463" s="3" t="s">
         <v>3</v>
@@ -6898,7 +6916,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="12" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C464" s="3" t="s">
         <v>3</v>
@@ -6909,7 +6927,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C465" s="3" t="s">
         <v>3</v>
@@ -6920,7 +6938,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C466" s="3" t="s">
         <v>3</v>
@@ -6931,7 +6949,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C467" s="3" t="s">
         <v>3</v>
@@ -6942,7 +6960,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C468" s="3" t="s">
         <v>3</v>
@@ -6953,7 +6971,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C469" s="3" t="s">
         <v>3</v>
@@ -6964,7 +6982,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C470" s="3" t="s">
         <v>3</v>
@@ -6975,7 +6993,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C471" s="3" t="s">
         <v>3</v>
@@ -6986,49 +7004,49 @@
         <v>392</v>
       </c>
       <c r="B472" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="C472" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" ht="21">
+      <c r="A473" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B473" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="C473" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" ht="21">
+      <c r="A474" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B474" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="C472" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="473" spans="1:3" ht="21">
-      <c r="B473" s="13"/>
-      <c r="C473" s="3"/>
-    </row>
-    <row r="474" spans="1:3" ht="21">
-      <c r="A474" s="6"/>
-      <c r="B474" s="13"/>
-      <c r="C474" s="3"/>
+      <c r="C474" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="475" spans="1:3" ht="21">
-      <c r="A475" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B475" s="12" t="s">
-        <v>453</v>
-      </c>
-      <c r="C475" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B475" s="13"/>
+      <c r="C475" s="3"/>
     </row>
     <row r="476" spans="1:3" ht="21">
-      <c r="A476" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B476" s="12" t="s">
-        <v>454</v>
-      </c>
-      <c r="C476" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A476" s="6"/>
+      <c r="B476" s="13"/>
+      <c r="C476" s="3"/>
     </row>
     <row r="477" spans="1:3" ht="21">
       <c r="A477" s="4" t="s">
         <v>452</v>
       </c>
       <c r="B477" s="12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C477" s="3" t="s">
         <v>3</v>
@@ -7039,7 +7057,7 @@
         <v>452</v>
       </c>
       <c r="B478" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C478" s="3" t="s">
         <v>3</v>
@@ -7050,7 +7068,7 @@
         <v>452</v>
       </c>
       <c r="B479" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C479" s="3" t="s">
         <v>3</v>
@@ -7061,7 +7079,7 @@
         <v>452</v>
       </c>
       <c r="B480" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C480" s="3" t="s">
         <v>3</v>
@@ -7072,7 +7090,7 @@
         <v>452</v>
       </c>
       <c r="B481" s="12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C481" s="3" t="s">
         <v>3</v>
@@ -7083,7 +7101,7 @@
         <v>452</v>
       </c>
       <c r="B482" s="12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C482" s="3" t="s">
         <v>3</v>
@@ -7094,7 +7112,7 @@
         <v>452</v>
       </c>
       <c r="B483" s="12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C483" s="3" t="s">
         <v>3</v>
@@ -7105,17 +7123,33 @@
         <v>452</v>
       </c>
       <c r="B484" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="C484" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" ht="21">
+      <c r="A485" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B485" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="C485" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" ht="21">
+      <c r="A486" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B486" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="C484" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="485" spans="1:3">
-      <c r="B485" s="17"/>
-    </row>
-    <row r="486" spans="1:3">
-      <c r="B486" s="17"/>
+      <c r="C486" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="487" spans="1:3">
       <c r="B487" s="17"/>
@@ -7128,6 +7162,12 @@
     </row>
     <row r="490" spans="1:3">
       <c r="B490" s="17"/>
+    </row>
+    <row r="491" spans="1:3">
+      <c r="B491" s="17"/>
+    </row>
+    <row r="492" spans="1:3">
+      <c r="B492" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7226,361 +7266,363 @@
     <hyperlink ref="B106" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
     <hyperlink ref="B107" r:id="rId94"/>
     <hyperlink ref="B110" r:id="rId95"/>
-    <hyperlink ref="B112" r:id="rId96"/>
-    <hyperlink ref="B113" r:id="rId97"/>
-    <hyperlink ref="B114" r:id="rId98"/>
-    <hyperlink ref="B116" r:id="rId99"/>
-    <hyperlink ref="B117" r:id="rId100"/>
-    <hyperlink ref="B118" r:id="rId101"/>
-    <hyperlink ref="B119" r:id="rId102"/>
-    <hyperlink ref="B120" r:id="rId103"/>
-    <hyperlink ref="B121" r:id="rId104"/>
-    <hyperlink ref="B122" r:id="rId105"/>
-    <hyperlink ref="B123" r:id="rId106"/>
-    <hyperlink ref="B124" r:id="rId107"/>
-    <hyperlink ref="B125" r:id="rId108"/>
-    <hyperlink ref="B126" r:id="rId109"/>
-    <hyperlink ref="B127" r:id="rId110"/>
-    <hyperlink ref="B128" r:id="rId111"/>
-    <hyperlink ref="B129" r:id="rId112"/>
-    <hyperlink ref="B130" r:id="rId113"/>
-    <hyperlink ref="B131" r:id="rId114"/>
-    <hyperlink ref="B132" r:id="rId115"/>
-    <hyperlink ref="B133" r:id="rId116"/>
-    <hyperlink ref="B134" r:id="rId117"/>
-    <hyperlink ref="B135" r:id="rId118"/>
-    <hyperlink ref="B136" r:id="rId119"/>
-    <hyperlink ref="B137" r:id="rId120"/>
-    <hyperlink ref="B138" r:id="rId121"/>
-    <hyperlink ref="B139" r:id="rId122"/>
+    <hyperlink ref="B114" r:id="rId96"/>
+    <hyperlink ref="B115" r:id="rId97"/>
+    <hyperlink ref="B116" r:id="rId98"/>
+    <hyperlink ref="B118" r:id="rId99"/>
+    <hyperlink ref="B119" r:id="rId100"/>
+    <hyperlink ref="B120" r:id="rId101"/>
+    <hyperlink ref="B121" r:id="rId102"/>
+    <hyperlink ref="B122" r:id="rId103"/>
+    <hyperlink ref="B123" r:id="rId104"/>
+    <hyperlink ref="B124" r:id="rId105"/>
+    <hyperlink ref="B125" r:id="rId106"/>
+    <hyperlink ref="B126" r:id="rId107"/>
+    <hyperlink ref="B127" r:id="rId108"/>
+    <hyperlink ref="B128" r:id="rId109"/>
+    <hyperlink ref="B129" r:id="rId110"/>
+    <hyperlink ref="B130" r:id="rId111"/>
+    <hyperlink ref="B131" r:id="rId112"/>
+    <hyperlink ref="B132" r:id="rId113"/>
+    <hyperlink ref="B133" r:id="rId114"/>
+    <hyperlink ref="B134" r:id="rId115"/>
+    <hyperlink ref="B135" r:id="rId116"/>
+    <hyperlink ref="B136" r:id="rId117"/>
+    <hyperlink ref="B137" r:id="rId118"/>
+    <hyperlink ref="B138" r:id="rId119"/>
+    <hyperlink ref="B139" r:id="rId120"/>
+    <hyperlink ref="B140" r:id="rId121"/>
+    <hyperlink ref="B141" r:id="rId122"/>
     <hyperlink ref="B105" r:id="rId123"/>
-    <hyperlink ref="B115" r:id="rId124"/>
-    <hyperlink ref="B142" r:id="rId125"/>
-    <hyperlink ref="B143" r:id="rId126"/>
-    <hyperlink ref="B144" r:id="rId127"/>
-    <hyperlink ref="B145" r:id="rId128"/>
-    <hyperlink ref="B146" r:id="rId129"/>
-    <hyperlink ref="B147" r:id="rId130"/>
-    <hyperlink ref="B148" r:id="rId131"/>
-    <hyperlink ref="B149" r:id="rId132"/>
-    <hyperlink ref="B150" r:id="rId133"/>
-    <hyperlink ref="B151" r:id="rId134"/>
-    <hyperlink ref="B152" r:id="rId135"/>
-    <hyperlink ref="B153" r:id="rId136"/>
-    <hyperlink ref="B154" r:id="rId137"/>
-    <hyperlink ref="B155" r:id="rId138"/>
-    <hyperlink ref="B156" r:id="rId139"/>
-    <hyperlink ref="B157" r:id="rId140"/>
-    <hyperlink ref="B158" r:id="rId141"/>
-    <hyperlink ref="B159" r:id="rId142"/>
-    <hyperlink ref="B160" r:id="rId143"/>
-    <hyperlink ref="B161" r:id="rId144"/>
-    <hyperlink ref="B162" r:id="rId145"/>
-    <hyperlink ref="B163" r:id="rId146"/>
-    <hyperlink ref="B164" r:id="rId147"/>
-    <hyperlink ref="B165" r:id="rId148"/>
-    <hyperlink ref="B166" r:id="rId149"/>
-    <hyperlink ref="B169" r:id="rId150"/>
-    <hyperlink ref="B170" r:id="rId151"/>
-    <hyperlink ref="B171" r:id="rId152"/>
-    <hyperlink ref="B172" r:id="rId153"/>
-    <hyperlink ref="B173" r:id="rId154"/>
-    <hyperlink ref="B174" r:id="rId155"/>
-    <hyperlink ref="B175" r:id="rId156"/>
-    <hyperlink ref="B176" r:id="rId157"/>
-    <hyperlink ref="B177" r:id="rId158"/>
-    <hyperlink ref="B180" r:id="rId159"/>
-    <hyperlink ref="B181" r:id="rId160"/>
-    <hyperlink ref="B182" r:id="rId161"/>
-    <hyperlink ref="B183" r:id="rId162"/>
-    <hyperlink ref="B184" r:id="rId163"/>
-    <hyperlink ref="B185" r:id="rId164"/>
-    <hyperlink ref="B186" r:id="rId165"/>
-    <hyperlink ref="B187" r:id="rId166"/>
-    <hyperlink ref="B188" r:id="rId167"/>
-    <hyperlink ref="B189" r:id="rId168"/>
-    <hyperlink ref="B190" r:id="rId169"/>
-    <hyperlink ref="B191" r:id="rId170"/>
-    <hyperlink ref="B192" r:id="rId171"/>
-    <hyperlink ref="B193" r:id="rId172"/>
-    <hyperlink ref="B194" r:id="rId173"/>
-    <hyperlink ref="B195" r:id="rId174"/>
-    <hyperlink ref="B196" r:id="rId175"/>
-    <hyperlink ref="B197" r:id="rId176"/>
-    <hyperlink ref="B198" r:id="rId177"/>
-    <hyperlink ref="B199" r:id="rId178"/>
-    <hyperlink ref="B200" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
-    <hyperlink ref="B201" r:id="rId180"/>
-    <hyperlink ref="B202" r:id="rId181"/>
-    <hyperlink ref="B203" r:id="rId182"/>
-    <hyperlink ref="B204" r:id="rId183"/>
-    <hyperlink ref="B205" r:id="rId184"/>
-    <hyperlink ref="B206" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
-    <hyperlink ref="B207" r:id="rId186"/>
-    <hyperlink ref="B208" r:id="rId187"/>
-    <hyperlink ref="B209" r:id="rId188"/>
-    <hyperlink ref="B210" r:id="rId189"/>
-    <hyperlink ref="B211" r:id="rId190"/>
-    <hyperlink ref="B212" r:id="rId191"/>
-    <hyperlink ref="B213" r:id="rId192"/>
-    <hyperlink ref="B214" r:id="rId193"/>
-    <hyperlink ref="B217" r:id="rId194"/>
-    <hyperlink ref="B218" r:id="rId195"/>
-    <hyperlink ref="B219" r:id="rId196"/>
-    <hyperlink ref="B220" r:id="rId197"/>
-    <hyperlink ref="B221" r:id="rId198"/>
-    <hyperlink ref="B222" r:id="rId199"/>
-    <hyperlink ref="B223" r:id="rId200"/>
-    <hyperlink ref="B224" r:id="rId201"/>
-    <hyperlink ref="B225" r:id="rId202"/>
-    <hyperlink ref="B226" r:id="rId203"/>
-    <hyperlink ref="B227" r:id="rId204"/>
-    <hyperlink ref="B228" r:id="rId205"/>
-    <hyperlink ref="B229" r:id="rId206"/>
-    <hyperlink ref="B230" r:id="rId207"/>
-    <hyperlink ref="B231" r:id="rId208"/>
-    <hyperlink ref="B232" r:id="rId209"/>
-    <hyperlink ref="B233" r:id="rId210"/>
-    <hyperlink ref="B234" r:id="rId211"/>
-    <hyperlink ref="B235" r:id="rId212"/>
-    <hyperlink ref="B236" r:id="rId213"/>
-    <hyperlink ref="B237" r:id="rId214"/>
-    <hyperlink ref="B238" r:id="rId215"/>
-    <hyperlink ref="B241" r:id="rId216"/>
-    <hyperlink ref="B242" r:id="rId217"/>
-    <hyperlink ref="B243" r:id="rId218"/>
-    <hyperlink ref="B244" r:id="rId219"/>
-    <hyperlink ref="B245" r:id="rId220"/>
-    <hyperlink ref="B246" r:id="rId221"/>
-    <hyperlink ref="B247" r:id="rId222"/>
-    <hyperlink ref="B248" r:id="rId223"/>
-    <hyperlink ref="B249" r:id="rId224"/>
-    <hyperlink ref="B250" r:id="rId225"/>
-    <hyperlink ref="B251" r:id="rId226"/>
-    <hyperlink ref="B252" r:id="rId227"/>
-    <hyperlink ref="B253" r:id="rId228"/>
-    <hyperlink ref="B254" r:id="rId229"/>
-    <hyperlink ref="B255" r:id="rId230"/>
-    <hyperlink ref="B256" r:id="rId231"/>
-    <hyperlink ref="B257" r:id="rId232"/>
-    <hyperlink ref="B258" r:id="rId233"/>
-    <hyperlink ref="B259" r:id="rId234"/>
-    <hyperlink ref="B260" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B261" r:id="rId236"/>
-    <hyperlink ref="B262" r:id="rId237"/>
-    <hyperlink ref="B263" r:id="rId238"/>
-    <hyperlink ref="B264" r:id="rId239"/>
-    <hyperlink ref="B265" r:id="rId240"/>
-    <hyperlink ref="B266" r:id="rId241"/>
-    <hyperlink ref="B267" r:id="rId242"/>
-    <hyperlink ref="B268" r:id="rId243"/>
-    <hyperlink ref="B269" r:id="rId244"/>
-    <hyperlink ref="B270" r:id="rId245"/>
-    <hyperlink ref="B271" r:id="rId246"/>
-    <hyperlink ref="B272" r:id="rId247"/>
-    <hyperlink ref="B273" r:id="rId248"/>
-    <hyperlink ref="B274" r:id="rId249"/>
-    <hyperlink ref="B275" r:id="rId250"/>
-    <hyperlink ref="B278" r:id="rId251"/>
-    <hyperlink ref="B279" r:id="rId252"/>
-    <hyperlink ref="B280" r:id="rId253"/>
-    <hyperlink ref="B281" r:id="rId254"/>
-    <hyperlink ref="B282" r:id="rId255"/>
-    <hyperlink ref="B283" r:id="rId256"/>
-    <hyperlink ref="B284" r:id="rId257"/>
-    <hyperlink ref="B285" r:id="rId258"/>
-    <hyperlink ref="B286" r:id="rId259"/>
-    <hyperlink ref="B287" r:id="rId260"/>
-    <hyperlink ref="B288" r:id="rId261"/>
-    <hyperlink ref="B289" r:id="rId262"/>
-    <hyperlink ref="B290" r:id="rId263"/>
-    <hyperlink ref="B291" r:id="rId264"/>
-    <hyperlink ref="B292" r:id="rId265"/>
-    <hyperlink ref="B293" r:id="rId266"/>
-    <hyperlink ref="B294" r:id="rId267"/>
-    <hyperlink ref="B295" r:id="rId268"/>
-    <hyperlink ref="B296" r:id="rId269"/>
-    <hyperlink ref="B299" r:id="rId270"/>
-    <hyperlink ref="B300" r:id="rId271"/>
-    <hyperlink ref="B301" r:id="rId272"/>
-    <hyperlink ref="B302" r:id="rId273"/>
-    <hyperlink ref="B303" r:id="rId274"/>
-    <hyperlink ref="B304" r:id="rId275"/>
-    <hyperlink ref="B305" r:id="rId276"/>
-    <hyperlink ref="B306" r:id="rId277"/>
-    <hyperlink ref="B307" r:id="rId278"/>
-    <hyperlink ref="B308" r:id="rId279"/>
-    <hyperlink ref="B309" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
-    <hyperlink ref="B310" r:id="rId281"/>
-    <hyperlink ref="B311" r:id="rId282"/>
-    <hyperlink ref="B312" r:id="rId283"/>
-    <hyperlink ref="B313" r:id="rId284"/>
-    <hyperlink ref="B314" r:id="rId285"/>
-    <hyperlink ref="B315" r:id="rId286"/>
-    <hyperlink ref="B316" r:id="rId287"/>
-    <hyperlink ref="B317" r:id="rId288"/>
-    <hyperlink ref="B318" r:id="rId289"/>
-    <hyperlink ref="B319" r:id="rId290"/>
-    <hyperlink ref="B320" r:id="rId291"/>
-    <hyperlink ref="B321" r:id="rId292"/>
-    <hyperlink ref="B322" r:id="rId293"/>
-    <hyperlink ref="B323" r:id="rId294"/>
-    <hyperlink ref="B324" r:id="rId295"/>
-    <hyperlink ref="B325" r:id="rId296"/>
-    <hyperlink ref="B326" r:id="rId297"/>
-    <hyperlink ref="B327" r:id="rId298"/>
-    <hyperlink ref="B328" r:id="rId299"/>
-    <hyperlink ref="B329" r:id="rId300"/>
-    <hyperlink ref="B330" r:id="rId301"/>
-    <hyperlink ref="B331" r:id="rId302"/>
-    <hyperlink ref="B332" r:id="rId303"/>
-    <hyperlink ref="B333" r:id="rId304"/>
-    <hyperlink ref="B334" r:id="rId305"/>
-    <hyperlink ref="B335" r:id="rId306"/>
-    <hyperlink ref="B336" r:id="rId307"/>
-    <hyperlink ref="B339" r:id="rId308"/>
-    <hyperlink ref="B340" r:id="rId309"/>
-    <hyperlink ref="B341" r:id="rId310"/>
-    <hyperlink ref="B342" r:id="rId311"/>
-    <hyperlink ref="B343" r:id="rId312"/>
-    <hyperlink ref="B344" r:id="rId313"/>
-    <hyperlink ref="B345" r:id="rId314"/>
-    <hyperlink ref="B346" r:id="rId315"/>
-    <hyperlink ref="B347" r:id="rId316"/>
-    <hyperlink ref="B348" r:id="rId317"/>
-    <hyperlink ref="B349" r:id="rId318"/>
-    <hyperlink ref="B350" r:id="rId319"/>
-    <hyperlink ref="B351" r:id="rId320"/>
-    <hyperlink ref="B352" r:id="rId321"/>
-    <hyperlink ref="B353" r:id="rId322"/>
-    <hyperlink ref="B354" r:id="rId323"/>
-    <hyperlink ref="B355" r:id="rId324"/>
-    <hyperlink ref="B356" r:id="rId325"/>
-    <hyperlink ref="B360" r:id="rId326"/>
-    <hyperlink ref="B361" r:id="rId327"/>
-    <hyperlink ref="B362" r:id="rId328"/>
-    <hyperlink ref="B363" r:id="rId329"/>
-    <hyperlink ref="B364" r:id="rId330"/>
-    <hyperlink ref="B365" r:id="rId331"/>
-    <hyperlink ref="B366" r:id="rId332"/>
-    <hyperlink ref="B367" r:id="rId333"/>
-    <hyperlink ref="B368" r:id="rId334"/>
-    <hyperlink ref="B369" r:id="rId335"/>
-    <hyperlink ref="B370" r:id="rId336"/>
-    <hyperlink ref="B371" r:id="rId337"/>
-    <hyperlink ref="B372" r:id="rId338"/>
-    <hyperlink ref="B373" r:id="rId339"/>
-    <hyperlink ref="B374" r:id="rId340"/>
-    <hyperlink ref="B375" r:id="rId341"/>
-    <hyperlink ref="B376" r:id="rId342"/>
-    <hyperlink ref="B377" r:id="rId343"/>
-    <hyperlink ref="B378" r:id="rId344"/>
-    <hyperlink ref="B379" r:id="rId345"/>
-    <hyperlink ref="B380" r:id="rId346"/>
-    <hyperlink ref="B381" r:id="rId347"/>
-    <hyperlink ref="B382" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B383" r:id="rId349"/>
-    <hyperlink ref="B384" r:id="rId350"/>
-    <hyperlink ref="B385" r:id="rId351"/>
-    <hyperlink ref="B386" r:id="rId352"/>
-    <hyperlink ref="B387" r:id="rId353"/>
-    <hyperlink ref="B388" r:id="rId354"/>
-    <hyperlink ref="B389" r:id="rId355"/>
-    <hyperlink ref="B390" r:id="rId356"/>
-    <hyperlink ref="B391" r:id="rId357"/>
-    <hyperlink ref="B392" r:id="rId358"/>
-    <hyperlink ref="B393" r:id="rId359"/>
-    <hyperlink ref="B394" r:id="rId360"/>
-    <hyperlink ref="B395" r:id="rId361"/>
-    <hyperlink ref="B396" r:id="rId362"/>
-    <hyperlink ref="B397" r:id="rId363"/>
-    <hyperlink ref="B399" r:id="rId364"/>
-    <hyperlink ref="B398" r:id="rId365"/>
-    <hyperlink ref="B400" r:id="rId366"/>
-    <hyperlink ref="B401" r:id="rId367"/>
-    <hyperlink ref="B402" r:id="rId368"/>
-    <hyperlink ref="B405" r:id="rId369"/>
-    <hyperlink ref="B406" r:id="rId370"/>
-    <hyperlink ref="B407" r:id="rId371"/>
-    <hyperlink ref="B408" r:id="rId372"/>
-    <hyperlink ref="B409" r:id="rId373"/>
-    <hyperlink ref="B410" r:id="rId374"/>
-    <hyperlink ref="B413" r:id="rId375"/>
-    <hyperlink ref="B414" r:id="rId376"/>
-    <hyperlink ref="B415" r:id="rId377"/>
-    <hyperlink ref="B416" r:id="rId378"/>
-    <hyperlink ref="B417" r:id="rId379"/>
-    <hyperlink ref="B418" r:id="rId380"/>
-    <hyperlink ref="B419" r:id="rId381"/>
-    <hyperlink ref="B420" r:id="rId382"/>
-    <hyperlink ref="B421" r:id="rId383"/>
-    <hyperlink ref="B422" r:id="rId384"/>
-    <hyperlink ref="B423" r:id="rId385"/>
-    <hyperlink ref="B424" r:id="rId386"/>
-    <hyperlink ref="B425" r:id="rId387"/>
-    <hyperlink ref="B426" r:id="rId388"/>
-    <hyperlink ref="B427" r:id="rId389"/>
-    <hyperlink ref="B428" r:id="rId390"/>
-    <hyperlink ref="B429" r:id="rId391"/>
-    <hyperlink ref="B430" r:id="rId392"/>
-    <hyperlink ref="B431" r:id="rId393"/>
-    <hyperlink ref="B432" r:id="rId394"/>
-    <hyperlink ref="B433" r:id="rId395"/>
-    <hyperlink ref="B434" r:id="rId396"/>
-    <hyperlink ref="B435" r:id="rId397"/>
-    <hyperlink ref="B436" r:id="rId398"/>
-    <hyperlink ref="B437" r:id="rId399"/>
-    <hyperlink ref="B438" r:id="rId400"/>
-    <hyperlink ref="B439" r:id="rId401"/>
-    <hyperlink ref="B440" r:id="rId402"/>
-    <hyperlink ref="B441" r:id="rId403"/>
-    <hyperlink ref="B442" r:id="rId404"/>
-    <hyperlink ref="B443" r:id="rId405"/>
-    <hyperlink ref="B444" r:id="rId406"/>
-    <hyperlink ref="B445" r:id="rId407"/>
-    <hyperlink ref="B446" r:id="rId408"/>
-    <hyperlink ref="B447" r:id="rId409"/>
-    <hyperlink ref="B448" r:id="rId410"/>
-    <hyperlink ref="B449" r:id="rId411"/>
-    <hyperlink ref="B450" r:id="rId412"/>
-    <hyperlink ref="B451" r:id="rId413"/>
-    <hyperlink ref="B452" r:id="rId414"/>
-    <hyperlink ref="B454" r:id="rId415"/>
-    <hyperlink ref="B453" r:id="rId416"/>
-    <hyperlink ref="B455" r:id="rId417"/>
-    <hyperlink ref="B456" r:id="rId418"/>
-    <hyperlink ref="B457" r:id="rId419"/>
-    <hyperlink ref="B458" r:id="rId420"/>
-    <hyperlink ref="B459" r:id="rId421"/>
-    <hyperlink ref="B460" r:id="rId422"/>
-    <hyperlink ref="B461" r:id="rId423"/>
-    <hyperlink ref="B462" r:id="rId424"/>
-    <hyperlink ref="B463" r:id="rId425"/>
-    <hyperlink ref="B464" r:id="rId426"/>
-    <hyperlink ref="B465" r:id="rId427"/>
-    <hyperlink ref="B472" r:id="rId428"/>
-    <hyperlink ref="B471" r:id="rId429"/>
-    <hyperlink ref="B470" r:id="rId430"/>
-    <hyperlink ref="B469" r:id="rId431"/>
-    <hyperlink ref="B468" r:id="rId432"/>
-    <hyperlink ref="B467" r:id="rId433"/>
-    <hyperlink ref="B466" r:id="rId434"/>
-    <hyperlink ref="B475" r:id="rId435"/>
-    <hyperlink ref="B476" r:id="rId436"/>
-    <hyperlink ref="B477" r:id="rId437"/>
-    <hyperlink ref="B478" r:id="rId438"/>
-    <hyperlink ref="B479" r:id="rId439"/>
-    <hyperlink ref="B480" r:id="rId440"/>
-    <hyperlink ref="B481" r:id="rId441"/>
-    <hyperlink ref="B484" r:id="rId442"/>
-    <hyperlink ref="B482" r:id="rId443"/>
-    <hyperlink ref="B483" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B359" r:id="rId445"/>
+    <hyperlink ref="B117" r:id="rId124"/>
+    <hyperlink ref="B144" r:id="rId125"/>
+    <hyperlink ref="B145" r:id="rId126"/>
+    <hyperlink ref="B146" r:id="rId127"/>
+    <hyperlink ref="B147" r:id="rId128"/>
+    <hyperlink ref="B148" r:id="rId129"/>
+    <hyperlink ref="B149" r:id="rId130"/>
+    <hyperlink ref="B150" r:id="rId131"/>
+    <hyperlink ref="B151" r:id="rId132"/>
+    <hyperlink ref="B152" r:id="rId133"/>
+    <hyperlink ref="B153" r:id="rId134"/>
+    <hyperlink ref="B154" r:id="rId135"/>
+    <hyperlink ref="B155" r:id="rId136"/>
+    <hyperlink ref="B156" r:id="rId137"/>
+    <hyperlink ref="B157" r:id="rId138"/>
+    <hyperlink ref="B158" r:id="rId139"/>
+    <hyperlink ref="B159" r:id="rId140"/>
+    <hyperlink ref="B160" r:id="rId141"/>
+    <hyperlink ref="B161" r:id="rId142"/>
+    <hyperlink ref="B162" r:id="rId143"/>
+    <hyperlink ref="B163" r:id="rId144"/>
+    <hyperlink ref="B164" r:id="rId145"/>
+    <hyperlink ref="B165" r:id="rId146"/>
+    <hyperlink ref="B166" r:id="rId147"/>
+    <hyperlink ref="B167" r:id="rId148"/>
+    <hyperlink ref="B168" r:id="rId149"/>
+    <hyperlink ref="B171" r:id="rId150"/>
+    <hyperlink ref="B172" r:id="rId151"/>
+    <hyperlink ref="B173" r:id="rId152"/>
+    <hyperlink ref="B174" r:id="rId153"/>
+    <hyperlink ref="B175" r:id="rId154"/>
+    <hyperlink ref="B176" r:id="rId155"/>
+    <hyperlink ref="B177" r:id="rId156"/>
+    <hyperlink ref="B178" r:id="rId157"/>
+    <hyperlink ref="B179" r:id="rId158"/>
+    <hyperlink ref="B182" r:id="rId159"/>
+    <hyperlink ref="B183" r:id="rId160"/>
+    <hyperlink ref="B184" r:id="rId161"/>
+    <hyperlink ref="B185" r:id="rId162"/>
+    <hyperlink ref="B186" r:id="rId163"/>
+    <hyperlink ref="B187" r:id="rId164"/>
+    <hyperlink ref="B188" r:id="rId165"/>
+    <hyperlink ref="B189" r:id="rId166"/>
+    <hyperlink ref="B190" r:id="rId167"/>
+    <hyperlink ref="B191" r:id="rId168"/>
+    <hyperlink ref="B192" r:id="rId169"/>
+    <hyperlink ref="B193" r:id="rId170"/>
+    <hyperlink ref="B194" r:id="rId171"/>
+    <hyperlink ref="B195" r:id="rId172"/>
+    <hyperlink ref="B196" r:id="rId173"/>
+    <hyperlink ref="B197" r:id="rId174"/>
+    <hyperlink ref="B198" r:id="rId175"/>
+    <hyperlink ref="B199" r:id="rId176"/>
+    <hyperlink ref="B200" r:id="rId177"/>
+    <hyperlink ref="B201" r:id="rId178"/>
+    <hyperlink ref="B202" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
+    <hyperlink ref="B203" r:id="rId180"/>
+    <hyperlink ref="B204" r:id="rId181"/>
+    <hyperlink ref="B205" r:id="rId182"/>
+    <hyperlink ref="B206" r:id="rId183"/>
+    <hyperlink ref="B207" r:id="rId184"/>
+    <hyperlink ref="B208" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
+    <hyperlink ref="B209" r:id="rId186"/>
+    <hyperlink ref="B210" r:id="rId187"/>
+    <hyperlink ref="B211" r:id="rId188"/>
+    <hyperlink ref="B212" r:id="rId189"/>
+    <hyperlink ref="B213" r:id="rId190"/>
+    <hyperlink ref="B214" r:id="rId191"/>
+    <hyperlink ref="B215" r:id="rId192"/>
+    <hyperlink ref="B216" r:id="rId193"/>
+    <hyperlink ref="B219" r:id="rId194"/>
+    <hyperlink ref="B220" r:id="rId195"/>
+    <hyperlink ref="B221" r:id="rId196"/>
+    <hyperlink ref="B222" r:id="rId197"/>
+    <hyperlink ref="B223" r:id="rId198"/>
+    <hyperlink ref="B224" r:id="rId199"/>
+    <hyperlink ref="B225" r:id="rId200"/>
+    <hyperlink ref="B226" r:id="rId201"/>
+    <hyperlink ref="B227" r:id="rId202"/>
+    <hyperlink ref="B228" r:id="rId203"/>
+    <hyperlink ref="B229" r:id="rId204"/>
+    <hyperlink ref="B230" r:id="rId205"/>
+    <hyperlink ref="B231" r:id="rId206"/>
+    <hyperlink ref="B232" r:id="rId207"/>
+    <hyperlink ref="B233" r:id="rId208"/>
+    <hyperlink ref="B234" r:id="rId209"/>
+    <hyperlink ref="B235" r:id="rId210"/>
+    <hyperlink ref="B236" r:id="rId211"/>
+    <hyperlink ref="B237" r:id="rId212"/>
+    <hyperlink ref="B238" r:id="rId213"/>
+    <hyperlink ref="B239" r:id="rId214"/>
+    <hyperlink ref="B240" r:id="rId215"/>
+    <hyperlink ref="B243" r:id="rId216"/>
+    <hyperlink ref="B244" r:id="rId217"/>
+    <hyperlink ref="B245" r:id="rId218"/>
+    <hyperlink ref="B246" r:id="rId219"/>
+    <hyperlink ref="B247" r:id="rId220"/>
+    <hyperlink ref="B248" r:id="rId221"/>
+    <hyperlink ref="B249" r:id="rId222"/>
+    <hyperlink ref="B250" r:id="rId223"/>
+    <hyperlink ref="B251" r:id="rId224"/>
+    <hyperlink ref="B252" r:id="rId225"/>
+    <hyperlink ref="B253" r:id="rId226"/>
+    <hyperlink ref="B254" r:id="rId227"/>
+    <hyperlink ref="B255" r:id="rId228"/>
+    <hyperlink ref="B256" r:id="rId229"/>
+    <hyperlink ref="B257" r:id="rId230"/>
+    <hyperlink ref="B258" r:id="rId231"/>
+    <hyperlink ref="B259" r:id="rId232"/>
+    <hyperlink ref="B260" r:id="rId233"/>
+    <hyperlink ref="B261" r:id="rId234"/>
+    <hyperlink ref="B262" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B263" r:id="rId236"/>
+    <hyperlink ref="B264" r:id="rId237"/>
+    <hyperlink ref="B265" r:id="rId238"/>
+    <hyperlink ref="B266" r:id="rId239"/>
+    <hyperlink ref="B267" r:id="rId240"/>
+    <hyperlink ref="B268" r:id="rId241"/>
+    <hyperlink ref="B269" r:id="rId242"/>
+    <hyperlink ref="B270" r:id="rId243"/>
+    <hyperlink ref="B271" r:id="rId244"/>
+    <hyperlink ref="B272" r:id="rId245"/>
+    <hyperlink ref="B273" r:id="rId246"/>
+    <hyperlink ref="B274" r:id="rId247"/>
+    <hyperlink ref="B275" r:id="rId248"/>
+    <hyperlink ref="B276" r:id="rId249"/>
+    <hyperlink ref="B277" r:id="rId250"/>
+    <hyperlink ref="B280" r:id="rId251"/>
+    <hyperlink ref="B281" r:id="rId252"/>
+    <hyperlink ref="B282" r:id="rId253"/>
+    <hyperlink ref="B283" r:id="rId254"/>
+    <hyperlink ref="B284" r:id="rId255"/>
+    <hyperlink ref="B285" r:id="rId256"/>
+    <hyperlink ref="B286" r:id="rId257"/>
+    <hyperlink ref="B287" r:id="rId258"/>
+    <hyperlink ref="B288" r:id="rId259"/>
+    <hyperlink ref="B289" r:id="rId260"/>
+    <hyperlink ref="B290" r:id="rId261"/>
+    <hyperlink ref="B291" r:id="rId262"/>
+    <hyperlink ref="B292" r:id="rId263"/>
+    <hyperlink ref="B293" r:id="rId264"/>
+    <hyperlink ref="B294" r:id="rId265"/>
+    <hyperlink ref="B295" r:id="rId266"/>
+    <hyperlink ref="B296" r:id="rId267"/>
+    <hyperlink ref="B297" r:id="rId268"/>
+    <hyperlink ref="B298" r:id="rId269"/>
+    <hyperlink ref="B301" r:id="rId270"/>
+    <hyperlink ref="B302" r:id="rId271"/>
+    <hyperlink ref="B303" r:id="rId272"/>
+    <hyperlink ref="B304" r:id="rId273"/>
+    <hyperlink ref="B305" r:id="rId274"/>
+    <hyperlink ref="B306" r:id="rId275"/>
+    <hyperlink ref="B307" r:id="rId276"/>
+    <hyperlink ref="B308" r:id="rId277"/>
+    <hyperlink ref="B309" r:id="rId278"/>
+    <hyperlink ref="B310" r:id="rId279"/>
+    <hyperlink ref="B311" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B312" r:id="rId281"/>
+    <hyperlink ref="B313" r:id="rId282"/>
+    <hyperlink ref="B314" r:id="rId283"/>
+    <hyperlink ref="B315" r:id="rId284"/>
+    <hyperlink ref="B316" r:id="rId285"/>
+    <hyperlink ref="B317" r:id="rId286"/>
+    <hyperlink ref="B318" r:id="rId287"/>
+    <hyperlink ref="B319" r:id="rId288"/>
+    <hyperlink ref="B320" r:id="rId289"/>
+    <hyperlink ref="B321" r:id="rId290"/>
+    <hyperlink ref="B322" r:id="rId291"/>
+    <hyperlink ref="B323" r:id="rId292"/>
+    <hyperlink ref="B324" r:id="rId293"/>
+    <hyperlink ref="B325" r:id="rId294"/>
+    <hyperlink ref="B326" r:id="rId295"/>
+    <hyperlink ref="B327" r:id="rId296"/>
+    <hyperlink ref="B328" r:id="rId297"/>
+    <hyperlink ref="B329" r:id="rId298"/>
+    <hyperlink ref="B330" r:id="rId299"/>
+    <hyperlink ref="B331" r:id="rId300"/>
+    <hyperlink ref="B332" r:id="rId301"/>
+    <hyperlink ref="B333" r:id="rId302"/>
+    <hyperlink ref="B334" r:id="rId303"/>
+    <hyperlink ref="B335" r:id="rId304"/>
+    <hyperlink ref="B336" r:id="rId305"/>
+    <hyperlink ref="B337" r:id="rId306"/>
+    <hyperlink ref="B338" r:id="rId307"/>
+    <hyperlink ref="B341" r:id="rId308"/>
+    <hyperlink ref="B342" r:id="rId309"/>
+    <hyperlink ref="B343" r:id="rId310"/>
+    <hyperlink ref="B344" r:id="rId311"/>
+    <hyperlink ref="B345" r:id="rId312"/>
+    <hyperlink ref="B346" r:id="rId313"/>
+    <hyperlink ref="B347" r:id="rId314"/>
+    <hyperlink ref="B348" r:id="rId315"/>
+    <hyperlink ref="B349" r:id="rId316"/>
+    <hyperlink ref="B350" r:id="rId317"/>
+    <hyperlink ref="B351" r:id="rId318"/>
+    <hyperlink ref="B352" r:id="rId319"/>
+    <hyperlink ref="B353" r:id="rId320"/>
+    <hyperlink ref="B354" r:id="rId321"/>
+    <hyperlink ref="B355" r:id="rId322"/>
+    <hyperlink ref="B356" r:id="rId323"/>
+    <hyperlink ref="B357" r:id="rId324"/>
+    <hyperlink ref="B358" r:id="rId325"/>
+    <hyperlink ref="B362" r:id="rId326"/>
+    <hyperlink ref="B363" r:id="rId327"/>
+    <hyperlink ref="B364" r:id="rId328"/>
+    <hyperlink ref="B365" r:id="rId329"/>
+    <hyperlink ref="B366" r:id="rId330"/>
+    <hyperlink ref="B367" r:id="rId331"/>
+    <hyperlink ref="B368" r:id="rId332"/>
+    <hyperlink ref="B369" r:id="rId333"/>
+    <hyperlink ref="B370" r:id="rId334"/>
+    <hyperlink ref="B371" r:id="rId335"/>
+    <hyperlink ref="B372" r:id="rId336"/>
+    <hyperlink ref="B373" r:id="rId337"/>
+    <hyperlink ref="B374" r:id="rId338"/>
+    <hyperlink ref="B375" r:id="rId339"/>
+    <hyperlink ref="B376" r:id="rId340"/>
+    <hyperlink ref="B377" r:id="rId341"/>
+    <hyperlink ref="B378" r:id="rId342"/>
+    <hyperlink ref="B379" r:id="rId343"/>
+    <hyperlink ref="B380" r:id="rId344"/>
+    <hyperlink ref="B381" r:id="rId345"/>
+    <hyperlink ref="B382" r:id="rId346"/>
+    <hyperlink ref="B383" r:id="rId347"/>
+    <hyperlink ref="B384" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B385" r:id="rId349"/>
+    <hyperlink ref="B386" r:id="rId350"/>
+    <hyperlink ref="B387" r:id="rId351"/>
+    <hyperlink ref="B388" r:id="rId352"/>
+    <hyperlink ref="B389" r:id="rId353"/>
+    <hyperlink ref="B390" r:id="rId354"/>
+    <hyperlink ref="B391" r:id="rId355"/>
+    <hyperlink ref="B392" r:id="rId356"/>
+    <hyperlink ref="B393" r:id="rId357"/>
+    <hyperlink ref="B394" r:id="rId358"/>
+    <hyperlink ref="B395" r:id="rId359"/>
+    <hyperlink ref="B396" r:id="rId360"/>
+    <hyperlink ref="B397" r:id="rId361"/>
+    <hyperlink ref="B398" r:id="rId362"/>
+    <hyperlink ref="B399" r:id="rId363"/>
+    <hyperlink ref="B401" r:id="rId364"/>
+    <hyperlink ref="B400" r:id="rId365"/>
+    <hyperlink ref="B402" r:id="rId366"/>
+    <hyperlink ref="B403" r:id="rId367"/>
+    <hyperlink ref="B404" r:id="rId368"/>
+    <hyperlink ref="B407" r:id="rId369"/>
+    <hyperlink ref="B408" r:id="rId370"/>
+    <hyperlink ref="B409" r:id="rId371"/>
+    <hyperlink ref="B410" r:id="rId372"/>
+    <hyperlink ref="B411" r:id="rId373"/>
+    <hyperlink ref="B412" r:id="rId374"/>
+    <hyperlink ref="B415" r:id="rId375"/>
+    <hyperlink ref="B416" r:id="rId376"/>
+    <hyperlink ref="B417" r:id="rId377"/>
+    <hyperlink ref="B418" r:id="rId378"/>
+    <hyperlink ref="B419" r:id="rId379"/>
+    <hyperlink ref="B420" r:id="rId380"/>
+    <hyperlink ref="B421" r:id="rId381"/>
+    <hyperlink ref="B422" r:id="rId382"/>
+    <hyperlink ref="B423" r:id="rId383"/>
+    <hyperlink ref="B424" r:id="rId384"/>
+    <hyperlink ref="B425" r:id="rId385"/>
+    <hyperlink ref="B426" r:id="rId386"/>
+    <hyperlink ref="B427" r:id="rId387"/>
+    <hyperlink ref="B428" r:id="rId388"/>
+    <hyperlink ref="B429" r:id="rId389"/>
+    <hyperlink ref="B430" r:id="rId390"/>
+    <hyperlink ref="B431" r:id="rId391"/>
+    <hyperlink ref="B432" r:id="rId392"/>
+    <hyperlink ref="B433" r:id="rId393"/>
+    <hyperlink ref="B434" r:id="rId394"/>
+    <hyperlink ref="B435" r:id="rId395"/>
+    <hyperlink ref="B436" r:id="rId396"/>
+    <hyperlink ref="B437" r:id="rId397"/>
+    <hyperlink ref="B438" r:id="rId398"/>
+    <hyperlink ref="B439" r:id="rId399"/>
+    <hyperlink ref="B440" r:id="rId400"/>
+    <hyperlink ref="B441" r:id="rId401"/>
+    <hyperlink ref="B442" r:id="rId402"/>
+    <hyperlink ref="B443" r:id="rId403"/>
+    <hyperlink ref="B444" r:id="rId404"/>
+    <hyperlink ref="B445" r:id="rId405"/>
+    <hyperlink ref="B446" r:id="rId406"/>
+    <hyperlink ref="B447" r:id="rId407"/>
+    <hyperlink ref="B448" r:id="rId408"/>
+    <hyperlink ref="B449" r:id="rId409"/>
+    <hyperlink ref="B450" r:id="rId410"/>
+    <hyperlink ref="B451" r:id="rId411"/>
+    <hyperlink ref="B452" r:id="rId412"/>
+    <hyperlink ref="B453" r:id="rId413"/>
+    <hyperlink ref="B454" r:id="rId414"/>
+    <hyperlink ref="B456" r:id="rId415"/>
+    <hyperlink ref="B455" r:id="rId416"/>
+    <hyperlink ref="B457" r:id="rId417"/>
+    <hyperlink ref="B458" r:id="rId418"/>
+    <hyperlink ref="B459" r:id="rId419"/>
+    <hyperlink ref="B460" r:id="rId420"/>
+    <hyperlink ref="B461" r:id="rId421"/>
+    <hyperlink ref="B462" r:id="rId422"/>
+    <hyperlink ref="B463" r:id="rId423"/>
+    <hyperlink ref="B464" r:id="rId424"/>
+    <hyperlink ref="B465" r:id="rId425"/>
+    <hyperlink ref="B466" r:id="rId426"/>
+    <hyperlink ref="B467" r:id="rId427"/>
+    <hyperlink ref="B474" r:id="rId428"/>
+    <hyperlink ref="B473" r:id="rId429"/>
+    <hyperlink ref="B472" r:id="rId430"/>
+    <hyperlink ref="B471" r:id="rId431"/>
+    <hyperlink ref="B470" r:id="rId432"/>
+    <hyperlink ref="B469" r:id="rId433"/>
+    <hyperlink ref="B468" r:id="rId434"/>
+    <hyperlink ref="B477" r:id="rId435"/>
+    <hyperlink ref="B478" r:id="rId436"/>
+    <hyperlink ref="B479" r:id="rId437"/>
+    <hyperlink ref="B480" r:id="rId438"/>
+    <hyperlink ref="B481" r:id="rId439"/>
+    <hyperlink ref="B482" r:id="rId440"/>
+    <hyperlink ref="B483" r:id="rId441"/>
+    <hyperlink ref="B486" r:id="rId442"/>
+    <hyperlink ref="B484" r:id="rId443"/>
+    <hyperlink ref="B485" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B361" r:id="rId445"/>
     <hyperlink ref="B109" r:id="rId446"/>
-    <hyperlink ref="B111" r:id="rId447"/>
+    <hyperlink ref="B112" r:id="rId447"/>
+    <hyperlink ref="B111" r:id="rId448"/>
+    <hyperlink ref="B113" r:id="rId449"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId448"/>
-  <legacyDrawing r:id="rId449"/>
+  <pageSetup orientation="portrait" r:id="rId450"/>
+  <legacyDrawing r:id="rId451"/>
 </worksheet>
 </file>
</xml_diff>